<commit_message>
Add more stats for data
Going to organize it more, but wanted to add averages for each day to compare the days
</commit_message>
<xml_diff>
--- a/Data/TheFINALS_Points.xlsx
+++ b/Data/TheFINALS_Points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GitHub\THE_FINALS-WorldTour-Calculator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A8ACA-93BA-4379-88DB-3B5C122BAB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84208F91-3327-4F13-88A7-14FBDDC303B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>Total Games</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>AGT</t>
+  </si>
+  <si>
+    <t>Matches</t>
   </si>
 </sst>
 </file>
@@ -783,7 +786,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,10 +962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9762EC57-E733-40D9-8A42-9901A7D36B8F}">
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,6 +1602,12 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
       <c r="O13">
         <f>SUM(November9[Points])</f>
         <v>71</v>
@@ -1624,6 +1633,14 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
+      <c r="H14">
+        <f>ROWS(November7[Points])</f>
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <f>November7[[#Totals],[Points]]/ROWS(November7[Points])</f>
+        <v>9.8333333333333339</v>
+      </c>
       <c r="O14" t="s">
         <v>21</v>
       </c>
@@ -1640,6 +1657,12 @@
         <f>INT(November9[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November9[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>3 hrs  52 mins</v>
       </c>
+      <c r="V14" t="s">
+        <v>22</v>
+      </c>
+      <c r="W14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1669,6 +1692,14 @@
         <f>November9[[#Totals],[Points]]/November9[[#Totals],[Playtime (Minutes)]]</f>
         <v>0.30603448275862066</v>
       </c>
+      <c r="V15">
+        <f>ROWS(November10[Points])</f>
+        <v>7</v>
+      </c>
+      <c r="W15">
+        <f>November10[[#Totals],[Points]]/ROWS(November10[Points])</f>
+        <v>19.142857142857142</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1683,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1695,8 +1726,14 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1708,8 +1745,16 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f>ROWS(November9[Points])</f>
+        <v>10</v>
+      </c>
+      <c r="P18">
+        <f>November9[[#Totals],[Points]]/ROWS(November9[Points])</f>
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1722,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1735,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -1748,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1761,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1774,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
@@ -1787,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>SUM(November6[Points])</f>
         <v>141</v>
@@ -1801,7 +1846,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1819,7 +1864,7 @@
         <v>7 hrs  25 mins</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>November6[[#Totals],[Playtime (Minutes)]]/November6[[#Totals],[Games]]</f>
         <v>13.088235294117647</v>
@@ -1835,6 +1880,24 @@
       <c r="D27">
         <f>November6[[#Totals],[Points]]/November6[[#Totals],[Playtime (Minutes)]]</f>
         <v>0.31685393258426964</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>ROWS(November6[Points])</f>
+        <v>22</v>
+      </c>
+      <c r="B30">
+        <f>November6[[#Totals],[Points]]/ROWS(November6[Points])</f>
+        <v>6.4090909090909092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more data and setup for new set.
</commit_message>
<xml_diff>
--- a/Data/TheFINALS_Points.xlsx
+++ b/Data/TheFINALS_Points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GitHub\THE_FINALS-WorldTour-Calculator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988837AB-3A7E-4F0C-B5D7-6C2A8F3E8968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885E8813-6EF5-4322-9C83-B181729B0DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="24">
   <si>
     <t>Total Games</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Matches</t>
+  </si>
+  <si>
+    <t>November 11th</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,18 +199,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="38">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -338,9 +355,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -357,8 +371,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C27E572-866D-47E4-922E-826821481817}" name="Totals" displayName="Totals" ref="A1:D6" totalsRowCount="1" headerRowDxfId="34">
-  <autoFilter ref="A1:D5" xr:uid="{4C27E572-866D-47E4-922E-826821481817}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C27E572-866D-47E4-922E-826821481817}" name="Totals" displayName="Totals" ref="A1:D7" totalsRowCount="1" headerRowDxfId="37">
+  <autoFilter ref="A1:D6" xr:uid="{4C27E572-866D-47E4-922E-826821481817}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -369,7 +383,7 @@
     <tableColumn id="1" xr3:uid="{F17A2C25-1331-45B7-93CA-58341B49862D}" name="Total Points" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Totals[Total Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{40664CBD-E414-475B-A65B-20BCE21DEF0B}" name="Total Games" totalsRowFunction="custom" dataDxfId="33">
+    <tableColumn id="2" xr3:uid="{40664CBD-E414-475B-A65B-20BCE21DEF0B}" name="Total Games" totalsRowFunction="custom" dataDxfId="0">
       <calculatedColumnFormula>November6[[#Totals],[Points]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(Totals[Total Games])</totalsRowFormula>
     </tableColumn>
@@ -382,7 +396,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}" name="Averages" displayName="Averages" ref="G1:J2" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}" name="Averages" displayName="Averages" ref="G1:J2" headerRowDxfId="36">
   <autoFilter ref="G1:J2" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -390,17 +404,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0AA5346B-236D-4E0F-BA60-5AB0FC09F6C3}" name="Average Game Time (AGT)" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="1" xr3:uid="{0AA5346B-236D-4E0F-BA60-5AB0FC09F6C3}" name="Average Game Time (AGT)" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Games]]</calculatedColumnFormula>
       <totalsRowFormula array="1">INT(Averages[Average Game Time (AGT)])&amp;" minutes"</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E04C1373-75E0-4A6C-A2C9-4AA9B2CD365B}" name="Points Per Game (PPG)" dataDxfId="29">
+    <tableColumn id="2" xr3:uid="{E04C1373-75E0-4A6C-A2C9-4AA9B2CD365B}" name="Points Per Game (PPG)" dataDxfId="33">
       <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Games]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{89B46B09-6052-4D3C-AAEC-F9A7E8580516}" name="Minutes Per Point (MPP)" dataDxfId="28">
+    <tableColumn id="4" xr3:uid="{89B46B09-6052-4D3C-AAEC-F9A7E8580516}" name="Minutes Per Point (MPP)" dataDxfId="32">
       <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Points]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{728FBC8B-7DB9-4E00-BB6D-2AFFBA13751D}" name="Points Per Minute (PPM)" dataDxfId="27">
+    <tableColumn id="3" xr3:uid="{728FBC8B-7DB9-4E00-BB6D-2AFFBA13751D}" name="Points Per Minute (PPM)" dataDxfId="31">
       <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Playtime (Minutes)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -409,7 +423,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}" name="November6" displayName="November6" ref="A2:E25" totalsRowCount="1" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}" name="November6" displayName="November6" ref="A2:E25" totalsRowCount="1" headerRowDxfId="30">
   <autoFilter ref="A2:E24" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -418,16 +432,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{366B94B4-B5FA-4886-9257-E9412E290946}" name="Points" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="1" xr3:uid="{366B94B4-B5FA-4886-9257-E9412E290946}" name="Points" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
       <totalsRowFormula>SUM(November6[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{73EA15C4-D270-483C-AF4F-24B0B93502DB}" name="Games" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="2" xr3:uid="{73EA15C4-D270-483C-AF4F-24B0B93502DB}" name="Games" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula array="1">_xlfn.IFS(November6[[#This Row],[Points]]=2, 1, November6[[#This Row],[Points]]=6, 2, November6[[#This Row],[Points]]=14, 3, November6[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November6[Games])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B3F474C8-DDEB-4DBF-A1DC-4AFC668AED9D}" name="Start Time" totalsRowDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{8665BCD7-C389-46C0-8A10-F495D85709FF}" name="End Time" totalsRowDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{5DE48718-2A9C-4594-A3FE-0C43DCAFF2C2}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="19">
+    <tableColumn id="4" xr3:uid="{B3F474C8-DDEB-4DBF-A1DC-4AFC668AED9D}" name="Start Time" totalsRowDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{8665BCD7-C389-46C0-8A10-F495D85709FF}" name="End Time" totalsRowDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{5DE48718-2A9C-4594-A3FE-0C43DCAFF2C2}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="23">
       <calculatedColumnFormula xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November6[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -437,7 +451,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}" name="November7" displayName="November7" ref="H2:L9" totalsRowCount="1" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}" name="November7" displayName="November7" ref="H2:L9" totalsRowCount="1" headerRowDxfId="22">
   <autoFilter ref="H2:L8" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -446,16 +460,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F89E074E-4750-48A3-A073-819989626FA6}" name="Points" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="1" xr3:uid="{F89E074E-4750-48A3-A073-819989626FA6}" name="Points" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <totalsRowFormula>SUM(November7[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D7CDB5A2-50B5-4939-8668-1785714D08C7}" name="Games" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="2" xr3:uid="{D7CDB5A2-50B5-4939-8668-1785714D08C7}" name="Games" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
       <calculatedColumnFormula array="1">_xlfn.IFS(November7[[#This Row],[Points]]=2, 1, November7[[#This Row],[Points]]=6, 2, November7[[#This Row],[Points]]=14, 3, November7[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November7[Games])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28309402-7EF3-454D-883F-D251D524A71A}" name="Start Time" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{74A71E4E-B89F-47C8-B7A2-E5012A8EEFF3}" name="End Time" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{5610F31C-E244-4937-8B69-B467C9F24C5D}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="11">
+    <tableColumn id="4" xr3:uid="{28309402-7EF3-454D-883F-D251D524A71A}" name="Start Time" totalsRowDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{74A71E4E-B89F-47C8-B7A2-E5012A8EEFF3}" name="End Time" totalsRowDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{5610F31C-E244-4937-8B69-B467C9F24C5D}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="15">
       <calculatedColumnFormula xml:space="preserve"> (INT(November7[[#This Row],[End Time]]/100)*60 + MOD(November7[[#This Row],[End Time]],100)) - (INT(November7[[#This Row],[Start Time]]/100)*60 + MOD(November7[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November7[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -465,7 +479,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}" name="November9" displayName="November9" ref="O2:S13" totalsRowCount="1" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}" name="November9" displayName="November9" ref="O2:S13" totalsRowCount="1" headerRowDxfId="14">
   <autoFilter ref="O2:S12" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -474,16 +488,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CDE914EB-DF9D-42C8-A121-6BDB5A6D584A}" name="Points" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="1" xr3:uid="{CDE914EB-DF9D-42C8-A121-6BDB5A6D584A}" name="Points" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
       <totalsRowFormula>SUM(November9[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{423C97EA-A31A-446C-BECE-2F0330150ABC}" name="Games" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="2" xr3:uid="{423C97EA-A31A-446C-BECE-2F0330150ABC}" name="Games" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula array="1">_xlfn.IFS(November9[[#This Row],[Points]]=2, 1, November9[[#This Row],[Points]]=6, 2, November9[[#This Row],[Points]]=14, 3, November9[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November9[Games])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C922EE3A-46E9-42C2-B0FC-BF56A61D0BD7}" name="Start Time" totalsRowDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{6E1643A5-7328-4CFF-9BB2-C0C48B9C9925}" name="End Time" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{F4DDC90C-E19C-46A6-93D1-39B9313C9028}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="3">
+    <tableColumn id="4" xr3:uid="{C922EE3A-46E9-42C2-B0FC-BF56A61D0BD7}" name="Start Time" totalsRowDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{6E1643A5-7328-4CFF-9BB2-C0C48B9C9925}" name="End Time" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{F4DDC90C-E19C-46A6-93D1-39B9313C9028}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="7">
       <calculatedColumnFormula xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November9[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -493,8 +507,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}" name="November10" displayName="November10" ref="V2:Z10" totalsRowCount="1" headerRowDxfId="2">
-  <autoFilter ref="V2:Z9" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}" name="November10" displayName="November10" ref="V2:Z11" totalsRowCount="1" headerRowDxfId="6">
+  <autoFilter ref="V2:Z10" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -502,10 +516,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{82DBC3F1-720E-42A7-9B61-D5995B025F92}" name="Points" totalsRowFunction="custom" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{82DBC3F1-720E-42A7-9B61-D5995B025F92}" name="Points" totalsRowFunction="custom" dataDxfId="2">
       <totalsRowFormula>SUM(November10[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D4B36161-B381-44F4-8DD1-C5FEFF82C827}" name="Games" totalsRowFunction="custom" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{D4B36161-B381-44F4-8DD1-C5FEFF82C827}" name="Games" totalsRowFunction="custom" dataDxfId="1">
       <calculatedColumnFormula array="1">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November10[Games])</totalsRowFormula>
     </tableColumn>
@@ -514,6 +528,34 @@
     <tableColumn id="6" xr3:uid="{F8ED1A20-4635-4A6C-8262-26D3B0886256}" name="Playtime (Minutes)" totalsRowFunction="custom">
       <calculatedColumnFormula xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November10[Playtime (Minutes)])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}" name="November11" displayName="November11" ref="AC2:AG4" totalsRowCount="1" headerRowDxfId="5">
+  <autoFilter ref="AC2:AG3" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{17F8BEAD-5484-4181-AD6E-07482D69DE92}" name="Points" totalsRowFunction="custom" dataDxfId="4">
+      <totalsRowFormula>SUM(November11[Points])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{B6CD6212-DA43-4D8D-86AB-D2A238A82270}" name="Games" totalsRowFunction="custom" dataDxfId="3">
+      <calculatedColumnFormula array="1">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
+      <totalsRowFormula>SUM(November11[Games])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{398AD5BB-5E5F-4DE7-A1C9-5C90562A08F8}" name="Start Time"/>
+    <tableColumn id="5" xr3:uid="{681F54AF-8DAF-4DFE-8FBC-A274A6DB355A}" name="End Time"/>
+    <tableColumn id="6" xr3:uid="{99CB9CF4-605E-4FB4-A631-BF5DB7AAAD86}" name="Playtime (Minutes)" totalsRowFunction="custom">
+      <calculatedColumnFormula xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</calculatedColumnFormula>
+      <totalsRowFormula>SUM(November11[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
@@ -783,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +878,7 @@
         <v>141</v>
       </c>
       <c r="C2">
-        <f>November6[[#Totals],[Games]]</f>
+        <f>IFERROR(November6[[#Totals],[Games]], 0)</f>
         <v>34</v>
       </c>
       <c r="D2">
@@ -845,19 +887,19 @@
       </c>
       <c r="G2" s="1">
         <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Games]]</f>
-        <v>12.752941176470589</v>
+        <v>12.693181818181818</v>
       </c>
       <c r="H2" s="1">
         <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Games]]</f>
-        <v>4.7647058823529411</v>
+        <v>4.8863636363636367</v>
       </c>
       <c r="I2" s="1">
         <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Points]]</f>
-        <v>2.6765432098765434</v>
+        <v>2.597674418604651</v>
       </c>
       <c r="J2" s="1">
         <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Playtime (Minutes)]]</f>
-        <v>0.37361623616236161</v>
+        <v>0.38495971351835273</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -869,7 +911,7 @@
         <v>59</v>
       </c>
       <c r="C3">
-        <f>November7[[#Totals],[Games]]</f>
+        <f>IFERROR(November7[[#Totals],[Games]], 0)</f>
         <v>13</v>
       </c>
       <c r="D3">
@@ -894,7 +936,7 @@
         <v>71</v>
       </c>
       <c r="C4">
-        <f>November9[[#Totals],[Games]]</f>
+        <f>IFERROR(November9[[#Totals],[Games]], 0)</f>
         <v>18</v>
       </c>
       <c r="D4">
@@ -908,38 +950,55 @@
       </c>
       <c r="B5">
         <f>November10[[#Totals],[Points]]</f>
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="C5">
         <f>IFERROR(November10[[#Totals],[Games]], 0)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <f>November10[[#Totals],[Playtime (Minutes)]]</f>
-        <v>238</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
+      <c r="A6" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B6">
+        <f>November11[[#Totals],[Points]]</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <f>IFERROR(November11[[#Totals],[Games]], 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>November11[[#Totals],[Playtime (Minutes)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <f>SUM(Totals[Total Points])</f>
-        <v>405</v>
-      </c>
-      <c r="C6">
+        <v>430</v>
+      </c>
+      <c r="C7">
         <f>SUM(Totals[Total Games])</f>
-        <v>85</v>
-      </c>
-      <c r="D6">
+        <v>88</v>
+      </c>
+      <c r="D7">
         <f>SUM(Totals[Total Playtime (Minutes)])</f>
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="str">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="str">
         <f>INT(Totals[[#Totals],[Total Playtime (Minutes)]]/60)&amp;" hours  "&amp;INT(MOD(Totals[[#Totals],[Total Playtime (Minutes)]],60))&amp;" minutes"</f>
-        <v>18 hours  4 minutes</v>
+        <v>18 hours  37 minutes</v>
       </c>
     </row>
   </sheetData>
@@ -948,10 +1007,11 @@
     <hyperlink ref="A3" location="DailyData!H1" display="November 7th" xr:uid="{AC8FC688-EBC1-4712-8089-FEE348D9964B}"/>
     <hyperlink ref="A4" location="DailyData!O1" display="November 9th" xr:uid="{9704D6B7-14DF-4C2C-BF93-C2230CF59ADA}"/>
     <hyperlink ref="A5" location="DailyData!V1" display="November 10th" xr:uid="{1B3FB756-63A6-46A9-8116-BFE00142D22A}"/>
+    <hyperlink ref="A6" location="DailyData!AC1" display="November 11th" xr:uid="{323360C2-27FA-4A82-B965-6C0D4578D900}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:C3 C4:C5" calculatedColumn="1"/>
+    <ignoredError sqref="C5:C6 C2:C4" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
@@ -962,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9762EC57-E733-40D9-8A42-9901A7D36B8F}">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,9 +1049,14 @@
     <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="23" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1020,8 +1085,15 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1082,8 +1154,23 @@
       <c r="Z2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1152,8 +1239,16 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>238</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AD3" t="e" cm="1">
+        <f t="array" ref="AD3">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AG3">
+        <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1199,19 +1294,37 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4">
         <v>25</v>
       </c>
-      <c r="W4" s="5" cm="1">
+      <c r="W4" cm="1">
         <f t="array" ref="W4">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
+      <c r="X4">
+        <v>2339</v>
+      </c>
+      <c r="Y4">
+        <v>2412</v>
+      </c>
       <c r="Z4">
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="AC4">
+        <f>SUM(November11[Points])</f>
+        <v>0</v>
+      </c>
+      <c r="AD4" t="e">
+        <f>SUM(November11[Games])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AG4">
+        <f>SUM(November11[Playtime (Minutes)])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
@@ -1245,10 +1358,10 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5">
         <v>25</v>
       </c>
-      <c r="W5" s="5" cm="1">
+      <c r="W5" cm="1">
         <f t="array" ref="W5">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
@@ -1256,8 +1369,24 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG5" s="1" t="str">
+        <f>INT(November11[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November11[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
+        <v>0 hrs  0 mins</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1291,10 +1420,10 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6">
         <v>25</v>
       </c>
-      <c r="W6" s="5" cm="1">
+      <c r="W6" cm="1">
         <f t="array" ref="W6">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
@@ -1302,8 +1431,24 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC6" t="e">
+        <f>November11[[#Totals],[Playtime (Minutes)]]/November11[[#Totals],[Games]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD6" t="e">
+        <f>November11[[#Totals],[Points]]/November11[[#Totals],[Games]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AE6" t="e">
+        <f>November11[[#Totals],[Playtime (Minutes)]]/November11[[#Totals],[Points]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF6" t="e">
+        <f>November11[[#Totals],[Points]]/November11[[#Totals],[Playtime (Minutes)]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14</v>
       </c>
@@ -1337,10 +1482,10 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7">
         <v>14</v>
       </c>
-      <c r="W7" s="5" cm="1">
+      <c r="W7" cm="1">
         <f t="array" ref="W7">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
@@ -1349,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1383,10 +1528,10 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8">
         <v>25</v>
       </c>
-      <c r="W8" s="5" cm="1">
+      <c r="W8" cm="1">
         <f t="array" ref="W8">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
@@ -1394,8 +1539,14 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1430,10 +1581,10 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9">
         <v>6</v>
       </c>
-      <c r="W9" s="5" cm="1">
+      <c r="W9" cm="1">
         <f t="array" ref="W9">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</f>
         <v>2</v>
       </c>
@@ -1441,8 +1592,16 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC9">
+        <f>ROWS(November11[Points])</f>
+        <v>1</v>
+      </c>
+      <c r="AD9">
+        <f>November11[[#Totals],[Points]]/ROWS(November11[Points])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1481,20 +1640,19 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V10">
-        <f>SUM(November10[Points])</f>
-        <v>134</v>
-      </c>
-      <c r="W10">
-        <f>SUM(November10[Games])</f>
-        <v>20</v>
+      <c r="V10" s="4">
+        <v>25</v>
+      </c>
+      <c r="W10" s="5" cm="1">
+        <f t="array" ref="W10">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
       </c>
       <c r="Z10">
-        <f>SUM(November10[Playtime (Minutes)])</f>
-        <v>238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+        <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1533,24 +1691,20 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V11" t="s">
-        <v>21</v>
-      </c>
-      <c r="W11" t="s">
-        <v>14</v>
-      </c>
-      <c r="X11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z11" s="1" t="str">
-        <f>INT(November10[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November10[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
-        <v>3 hrs  58 mins</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V11">
+        <f>SUM(November10[Points])</f>
+        <v>159</v>
+      </c>
+      <c r="W11">
+        <f>SUM(November10[Games])</f>
+        <v>23</v>
+      </c>
+      <c r="Z11">
+        <f>SUM(November10[Playtime (Minutes)])</f>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1573,24 +1727,24 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V12">
-        <f>November10[[#Totals],[Playtime (Minutes)]]/November10[[#Totals],[Games]]</f>
-        <v>11.9</v>
-      </c>
-      <c r="W12">
-        <f>November10[[#Totals],[Points]]/November10[[#Totals],[Games]]</f>
-        <v>6.7</v>
-      </c>
-      <c r="X12">
-        <f>November10[[#Totals],[Playtime (Minutes)]]/November10[[#Totals],[Points]]</f>
-        <v>1.7761194029850746</v>
-      </c>
-      <c r="Y12">
-        <f>November10[[#Totals],[Points]]/November10[[#Totals],[Playtime (Minutes)]]</f>
-        <v>0.56302521008403361</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W12" t="s">
+        <v>14</v>
+      </c>
+      <c r="X12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z12" s="1" t="str">
+        <f>INT(November10[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November10[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
+        <v>4 hrs  31 mins</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1620,8 +1774,24 @@
         <f>SUM(November9[Playtime (Minutes)])</f>
         <v>232</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V13">
+        <f>November10[[#Totals],[Playtime (Minutes)]]/November10[[#Totals],[Games]]</f>
+        <v>11.782608695652174</v>
+      </c>
+      <c r="W13">
+        <f>November10[[#Totals],[Points]]/November10[[#Totals],[Games]]</f>
+        <v>6.9130434782608692</v>
+      </c>
+      <c r="X13">
+        <f>November10[[#Totals],[Playtime (Minutes)]]/November10[[#Totals],[Points]]</f>
+        <v>1.7044025157232705</v>
+      </c>
+      <c r="Y13">
+        <f>November10[[#Totals],[Points]]/November10[[#Totals],[Playtime (Minutes)]]</f>
+        <v>0.58671586715867163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1657,14 +1827,8 @@
         <f>INT(November9[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November9[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>3 hrs  52 mins</v>
       </c>
-      <c r="V14" t="s">
-        <v>22</v>
-      </c>
-      <c r="W14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1692,16 +1856,14 @@
         <f>November9[[#Totals],[Points]]/November9[[#Totals],[Playtime (Minutes)]]</f>
         <v>0.30603448275862066</v>
       </c>
-      <c r="V15">
-        <f>ROWS(November10[Points])</f>
-        <v>7</v>
-      </c>
-      <c r="W15">
-        <f>November10[[#Totals],[Points]]/ROWS(November10[Points])</f>
-        <v>19.142857142857142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1712,6 +1874,14 @@
       <c r="E16">
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
+      </c>
+      <c r="V16">
+        <f>ROWS(November10[Points])</f>
+        <v>8</v>
+      </c>
+      <c r="W16">
+        <f>November10[[#Totals],[Points]]/ROWS(November10[Points])</f>
+        <v>19.875</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1901,20 +2071,22 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="O1:S1"/>
     <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AC1:AG1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more data and adjust wording on UI.
Plannig to overhaul games to rounds as technically it's rounds.
Assuming that a game is all the rounds played. Basically, you queue for a game, but you play multiple rounds per queue.
</commit_message>
<xml_diff>
--- a/Data/TheFINALS_Points.xlsx
+++ b/Data/TheFINALS_Points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GitHub\THE_FINALS-WorldTour-Calculator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885E8813-6EF5-4322-9C83-B181729B0DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059F0B9E-E004-46BE-977C-74EA9FB0A5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,7 +199,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -208,6 +207,13 @@
   <dxfs count="38">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -215,16 +221,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -353,6 +349,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -383,7 +382,7 @@
     <tableColumn id="1" xr3:uid="{F17A2C25-1331-45B7-93CA-58341B49862D}" name="Total Points" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Totals[Total Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{40664CBD-E414-475B-A65B-20BCE21DEF0B}" name="Total Games" totalsRowFunction="custom" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{40664CBD-E414-475B-A65B-20BCE21DEF0B}" name="Total Games" totalsRowFunction="custom" dataDxfId="36">
       <calculatedColumnFormula>November6[[#Totals],[Points]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(Totals[Total Games])</totalsRowFormula>
     </tableColumn>
@@ -396,7 +395,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}" name="Averages" displayName="Averages" ref="G1:J2" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}" name="Averages" displayName="Averages" ref="G1:J2" headerRowDxfId="35">
   <autoFilter ref="G1:J2" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -404,17 +403,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0AA5346B-236D-4E0F-BA60-5AB0FC09F6C3}" name="Average Game Time (AGT)" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="1" xr3:uid="{0AA5346B-236D-4E0F-BA60-5AB0FC09F6C3}" name="Average Game Time (AGT)" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="33">
       <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Games]]</calculatedColumnFormula>
       <totalsRowFormula array="1">INT(Averages[Average Game Time (AGT)])&amp;" minutes"</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E04C1373-75E0-4A6C-A2C9-4AA9B2CD365B}" name="Points Per Game (PPG)" dataDxfId="33">
+    <tableColumn id="2" xr3:uid="{E04C1373-75E0-4A6C-A2C9-4AA9B2CD365B}" name="Points Per Game (PPG)" dataDxfId="32">
       <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Games]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{89B46B09-6052-4D3C-AAEC-F9A7E8580516}" name="Minutes Per Point (MPP)" dataDxfId="32">
+    <tableColumn id="4" xr3:uid="{89B46B09-6052-4D3C-AAEC-F9A7E8580516}" name="Minutes Per Point (MPP)" dataDxfId="31">
       <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Points]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{728FBC8B-7DB9-4E00-BB6D-2AFFBA13751D}" name="Points Per Minute (PPM)" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{728FBC8B-7DB9-4E00-BB6D-2AFFBA13751D}" name="Points Per Minute (PPM)" dataDxfId="30">
       <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Playtime (Minutes)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -423,7 +422,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}" name="November6" displayName="November6" ref="A2:E25" totalsRowCount="1" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}" name="November6" displayName="November6" ref="A2:E25" totalsRowCount="1" headerRowDxfId="29">
   <autoFilter ref="A2:E24" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -432,16 +431,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{366B94B4-B5FA-4886-9257-E9412E290946}" name="Points" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="1" xr3:uid="{366B94B4-B5FA-4886-9257-E9412E290946}" name="Points" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="27">
       <totalsRowFormula>SUM(November6[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{73EA15C4-D270-483C-AF4F-24B0B93502DB}" name="Games" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="2" xr3:uid="{73EA15C4-D270-483C-AF4F-24B0B93502DB}" name="Games" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="25">
       <calculatedColumnFormula array="1">_xlfn.IFS(November6[[#This Row],[Points]]=2, 1, November6[[#This Row],[Points]]=6, 2, November6[[#This Row],[Points]]=14, 3, November6[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November6[Games])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B3F474C8-DDEB-4DBF-A1DC-4AFC668AED9D}" name="Start Time" totalsRowDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{8665BCD7-C389-46C0-8A10-F495D85709FF}" name="End Time" totalsRowDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{5DE48718-2A9C-4594-A3FE-0C43DCAFF2C2}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="23">
+    <tableColumn id="4" xr3:uid="{B3F474C8-DDEB-4DBF-A1DC-4AFC668AED9D}" name="Start Time" totalsRowDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{8665BCD7-C389-46C0-8A10-F495D85709FF}" name="End Time" totalsRowDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{5DE48718-2A9C-4594-A3FE-0C43DCAFF2C2}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="22">
       <calculatedColumnFormula xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November6[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -451,7 +450,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}" name="November7" displayName="November7" ref="H2:L9" totalsRowCount="1" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}" name="November7" displayName="November7" ref="H2:L9" totalsRowCount="1" headerRowDxfId="21">
   <autoFilter ref="H2:L8" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -460,16 +459,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F89E074E-4750-48A3-A073-819989626FA6}" name="Points" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
+    <tableColumn id="1" xr3:uid="{F89E074E-4750-48A3-A073-819989626FA6}" name="Points" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
       <totalsRowFormula>SUM(November7[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D7CDB5A2-50B5-4939-8668-1785714D08C7}" name="Games" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="2" xr3:uid="{D7CDB5A2-50B5-4939-8668-1785714D08C7}" name="Games" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula array="1">_xlfn.IFS(November7[[#This Row],[Points]]=2, 1, November7[[#This Row],[Points]]=6, 2, November7[[#This Row],[Points]]=14, 3, November7[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November7[Games])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28309402-7EF3-454D-883F-D251D524A71A}" name="Start Time" totalsRowDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{74A71E4E-B89F-47C8-B7A2-E5012A8EEFF3}" name="End Time" totalsRowDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{5610F31C-E244-4937-8B69-B467C9F24C5D}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="15">
+    <tableColumn id="4" xr3:uid="{28309402-7EF3-454D-883F-D251D524A71A}" name="Start Time" totalsRowDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{74A71E4E-B89F-47C8-B7A2-E5012A8EEFF3}" name="End Time" totalsRowDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{5610F31C-E244-4937-8B69-B467C9F24C5D}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="14">
       <calculatedColumnFormula xml:space="preserve"> (INT(November7[[#This Row],[End Time]]/100)*60 + MOD(November7[[#This Row],[End Time]],100)) - (INT(November7[[#This Row],[Start Time]]/100)*60 + MOD(November7[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November7[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -479,7 +478,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}" name="November9" displayName="November9" ref="O2:S13" totalsRowCount="1" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}" name="November9" displayName="November9" ref="O2:S13" totalsRowCount="1" headerRowDxfId="13">
   <autoFilter ref="O2:S12" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -488,16 +487,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CDE914EB-DF9D-42C8-A121-6BDB5A6D584A}" name="Points" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="1" xr3:uid="{CDE914EB-DF9D-42C8-A121-6BDB5A6D584A}" name="Points" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="11">
       <totalsRowFormula>SUM(November9[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{423C97EA-A31A-446C-BECE-2F0330150ABC}" name="Games" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="2" xr3:uid="{423C97EA-A31A-446C-BECE-2F0330150ABC}" name="Games" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula array="1">_xlfn.IFS(November9[[#This Row],[Points]]=2, 1, November9[[#This Row],[Points]]=6, 2, November9[[#This Row],[Points]]=14, 3, November9[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November9[Games])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C922EE3A-46E9-42C2-B0FC-BF56A61D0BD7}" name="Start Time" totalsRowDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{6E1643A5-7328-4CFF-9BB2-C0C48B9C9925}" name="End Time" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{F4DDC90C-E19C-46A6-93D1-39B9313C9028}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="7">
+    <tableColumn id="4" xr3:uid="{C922EE3A-46E9-42C2-B0FC-BF56A61D0BD7}" name="Start Time" totalsRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{6E1643A5-7328-4CFF-9BB2-C0C48B9C9925}" name="End Time" totalsRowDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{F4DDC90C-E19C-46A6-93D1-39B9313C9028}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="6">
       <calculatedColumnFormula xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November9[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -507,7 +506,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}" name="November10" displayName="November10" ref="V2:Z11" totalsRowCount="1" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}" name="November10" displayName="November10" ref="V2:Z11" totalsRowCount="1" headerRowDxfId="5">
   <autoFilter ref="V2:Z10" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -516,10 +515,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{82DBC3F1-720E-42A7-9B61-D5995B025F92}" name="Points" totalsRowFunction="custom" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{82DBC3F1-720E-42A7-9B61-D5995B025F92}" name="Points" totalsRowFunction="custom" dataDxfId="4">
       <totalsRowFormula>SUM(November10[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D4B36161-B381-44F4-8DD1-C5FEFF82C827}" name="Games" totalsRowFunction="custom" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{D4B36161-B381-44F4-8DD1-C5FEFF82C827}" name="Games" totalsRowFunction="custom" dataDxfId="3">
       <calculatedColumnFormula array="1">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November10[Games])</totalsRowFormula>
     </tableColumn>
@@ -535,8 +534,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}" name="November11" displayName="November11" ref="AC2:AG4" totalsRowCount="1" headerRowDxfId="5">
-  <autoFilter ref="AC2:AG3" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}" name="November11" displayName="November11" ref="AC2:AG7" totalsRowCount="1" headerRowDxfId="2">
+  <autoFilter ref="AC2:AG6" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -544,10 +543,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{17F8BEAD-5484-4181-AD6E-07482D69DE92}" name="Points" totalsRowFunction="custom" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{17F8BEAD-5484-4181-AD6E-07482D69DE92}" name="Points" totalsRowFunction="custom" dataDxfId="1">
       <totalsRowFormula>SUM(November11[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B6CD6212-DA43-4D8D-86AB-D2A238A82270}" name="Games" totalsRowFunction="custom" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{B6CD6212-DA43-4D8D-86AB-D2A238A82270}" name="Games" totalsRowFunction="custom" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November11[Games])</totalsRowFormula>
     </tableColumn>
@@ -828,7 +827,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,19 +886,19 @@
       </c>
       <c r="G2" s="1">
         <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Games]]</f>
-        <v>12.693181818181818</v>
+        <v>12.705263157894738</v>
       </c>
       <c r="H2" s="1">
         <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Games]]</f>
-        <v>4.8863636363636367</v>
+        <v>4.8947368421052628</v>
       </c>
       <c r="I2" s="1">
         <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Points]]</f>
-        <v>2.597674418604651</v>
+        <v>2.5956989247311828</v>
       </c>
       <c r="J2" s="1">
         <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Playtime (Minutes)]]</f>
-        <v>0.38495971351835273</v>
+        <v>0.38525269262634632</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -967,15 +966,15 @@
       </c>
       <c r="B6">
         <f>November11[[#Totals],[Points]]</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
+        <v>35</v>
+      </c>
+      <c r="C6">
         <f>IFERROR(November11[[#Totals],[Games]], 0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <f>November11[[#Totals],[Playtime (Minutes)]]</f>
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -984,21 +983,21 @@
       </c>
       <c r="B7">
         <f>SUM(Totals[Total Points])</f>
-        <v>430</v>
+        <v>465</v>
       </c>
       <c r="C7">
         <f>SUM(Totals[Total Games])</f>
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D7">
         <f>SUM(Totals[Total Playtime (Minutes)])</f>
-        <v>1117</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="str">
         <f>INT(Totals[[#Totals],[Total Playtime (Minutes)]]/60)&amp;" hours  "&amp;INT(MOD(Totals[[#Totals],[Total Playtime (Minutes)]],60))&amp;" minutes"</f>
-        <v>18 hours  37 minutes</v>
+        <v>20 hours  7 minutes</v>
       </c>
     </row>
   </sheetData>
@@ -1024,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9762EC57-E733-40D9-8A42-9901A7D36B8F}">
   <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AG1"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,13 +1238,22 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>238</v>
       </c>
-      <c r="AD3" t="e" cm="1">
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AD3" cm="1">
         <f t="array" ref="AD3">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</f>
-        <v>#N/A</v>
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1153</v>
+      </c>
+      <c r="AF3">
+        <v>1323</v>
       </c>
       <c r="AG3">
         <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -1311,16 +1319,15 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>33</v>
       </c>
-      <c r="AC4">
-        <f>SUM(November11[Points])</f>
-        <v>0</v>
-      </c>
-      <c r="AD4" t="e">
-        <f>SUM(November11[Games])</f>
-        <v>#N/A</v>
+      <c r="AC4" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="5" cm="1">
+        <f t="array" ref="AD4">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
       </c>
       <c r="AG4">
-        <f>SUM(November11[Playtime (Minutes)])</f>
+        <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
     </row>
@@ -1369,21 +1376,16 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="AC5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG5" s="1" t="str">
-        <f>INT(November11[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November11[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
-        <v>0 hrs  0 mins</v>
+      <c r="AC5" s="4">
+        <v>25</v>
+      </c>
+      <c r="AD5" s="5" cm="1">
+        <f t="array" ref="AD5">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AG5">
+        <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
@@ -1431,21 +1433,16 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="AC6" t="e">
-        <f>November11[[#Totals],[Playtime (Minutes)]]/November11[[#Totals],[Games]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD6" t="e">
-        <f>November11[[#Totals],[Points]]/November11[[#Totals],[Games]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AE6" t="e">
-        <f>November11[[#Totals],[Playtime (Minutes)]]/November11[[#Totals],[Points]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF6" t="e">
-        <f>November11[[#Totals],[Points]]/November11[[#Totals],[Playtime (Minutes)]]</f>
-        <v>#DIV/0!</v>
+      <c r="AC6" s="4">
+        <v>6</v>
+      </c>
+      <c r="AD6" s="5" cm="1">
+        <f t="array" ref="AD6">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AG6">
+        <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
@@ -1493,6 +1490,18 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
+      <c r="AC7">
+        <f>SUM(November11[Points])</f>
+        <v>35</v>
+      </c>
+      <c r="AD7">
+        <f>SUM(November11[Games])</f>
+        <v>7</v>
+      </c>
+      <c r="AG7">
+        <f>SUM(November11[Playtime (Minutes)])</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1540,10 +1549,20 @@
         <v>0</v>
       </c>
       <c r="AC8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AD8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF8" t="s">
         <v>16</v>
+      </c>
+      <c r="AG8" s="1" t="str">
+        <f>INT(November11[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November11[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
+        <v>1 hrs  30 mins</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
@@ -1593,12 +1612,20 @@
         <v>0</v>
       </c>
       <c r="AC9">
-        <f>ROWS(November11[Points])</f>
-        <v>1</v>
+        <f>November11[[#Totals],[Playtime (Minutes)]]/November11[[#Totals],[Games]]</f>
+        <v>12.857142857142858</v>
       </c>
       <c r="AD9">
-        <f>November11[[#Totals],[Points]]/ROWS(November11[Points])</f>
-        <v>0</v>
+        <f>November11[[#Totals],[Points]]/November11[[#Totals],[Games]]</f>
+        <v>5</v>
+      </c>
+      <c r="AE9">
+        <f>November11[[#Totals],[Playtime (Minutes)]]/November11[[#Totals],[Points]]</f>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="AF9">
+        <f>November11[[#Totals],[Points]]/November11[[#Totals],[Playtime (Minutes)]]</f>
+        <v>0.3888888888888889</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
@@ -1640,10 +1667,10 @@
         <f xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10">
         <v>25</v>
       </c>
-      <c r="W10" s="5" cm="1">
+      <c r="W10" cm="1">
         <f t="array" ref="W10">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
@@ -1703,6 +1730,12 @@
         <f>SUM(November10[Playtime (Minutes)])</f>
         <v>271</v>
       </c>
+      <c r="AC11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1742,6 +1775,14 @@
       <c r="Z12" s="1" t="str">
         <f>INT(November10[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November10[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>4 hrs  31 mins</v>
+      </c>
+      <c r="AC12">
+        <f>ROWS(November11[Points])</f>
+        <v>4</v>
+      </c>
+      <c r="AD12">
+        <f>November11[[#Totals],[Points]]/ROWS(November11[Points])</f>
+        <v>8.75</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More data and rename of fields
In data, instead of games it is now called rounds. Rounds is each round within a match.
</commit_message>
<xml_diff>
--- a/Data/TheFINALS_Points.xlsx
+++ b/Data/TheFINALS_Points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GitHub\THE_FINALS-WorldTour-Calculator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059F0B9E-E004-46BE-977C-74EA9FB0A5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673E1585-9EC4-4CDB-BB26-5714202D7679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -59,10 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="24">
-  <si>
-    <t>Total Games</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
   <si>
     <t>Total Points</t>
   </si>
@@ -85,9 +82,6 @@
     <t>Points</t>
   </si>
   <si>
-    <t>Games</t>
-  </si>
-  <si>
     <t>End Time</t>
   </si>
   <si>
@@ -103,34 +97,46 @@
     <t>Total Playtime (Minutes)</t>
   </si>
   <si>
-    <t>PPG</t>
-  </si>
-  <si>
     <t>MPP</t>
   </si>
   <si>
     <t>PPM</t>
   </si>
   <si>
-    <t>Average Game Time (AGT)</t>
-  </si>
-  <si>
-    <t>Points Per Game (PPG)</t>
-  </si>
-  <si>
     <t>Minutes Per Point (MPP)</t>
   </si>
   <si>
     <t>Points Per Minute (PPM)</t>
   </si>
   <si>
-    <t>AGT</t>
-  </si>
-  <si>
     <t>Matches</t>
   </si>
   <si>
     <t>November 11th</t>
+  </si>
+  <si>
+    <t>November 12th</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>Rounds</t>
+  </si>
+  <si>
+    <t>PPR</t>
+  </si>
+  <si>
+    <t>Total Rounds</t>
+  </si>
+  <si>
+    <t>Average Round Time (ART)</t>
+  </si>
+  <si>
+    <t>Points Per Round (PPR)</t>
+  </si>
+  <si>
+    <t>PPMatch</t>
   </si>
 </sst>
 </file>
@@ -188,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +203,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
@@ -204,7 +211,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="26">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -226,18 +236,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -245,22 +243,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -270,28 +253,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -351,9 +326,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -370,8 +342,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C27E572-866D-47E4-922E-826821481817}" name="Totals" displayName="Totals" ref="A1:D7" totalsRowCount="1" headerRowDxfId="37">
-  <autoFilter ref="A1:D6" xr:uid="{4C27E572-866D-47E4-922E-826821481817}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C27E572-866D-47E4-922E-826821481817}" name="Totals" displayName="Totals" ref="A1:D8" totalsRowCount="1" headerRowDxfId="25">
+  <autoFilter ref="A1:D7" xr:uid="{4C27E572-866D-47E4-922E-826821481817}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -382,9 +354,9 @@
     <tableColumn id="1" xr3:uid="{F17A2C25-1331-45B7-93CA-58341B49862D}" name="Total Points" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Totals[Total Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{40664CBD-E414-475B-A65B-20BCE21DEF0B}" name="Total Games" totalsRowFunction="custom" dataDxfId="36">
+    <tableColumn id="2" xr3:uid="{40664CBD-E414-475B-A65B-20BCE21DEF0B}" name="Total Rounds" totalsRowFunction="custom" dataDxfId="0">
       <calculatedColumnFormula>November6[[#Totals],[Points]]</calculatedColumnFormula>
-      <totalsRowFormula>SUM(Totals[Total Games])</totalsRowFormula>
+      <totalsRowFormula>SUM(Totals[Total Rounds])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C8AFE569-EB2B-4A94-8C17-1CF5EACFA5C3}" name="Total Playtime (Minutes)" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Totals[Total Playtime (Minutes)])</totalsRowFormula>
@@ -395,7 +367,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}" name="Averages" displayName="Averages" ref="G1:J2" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}" name="Averages" displayName="Averages" ref="G1:J2" headerRowDxfId="24">
   <autoFilter ref="G1:J2" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -403,17 +375,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0AA5346B-236D-4E0F-BA60-5AB0FC09F6C3}" name="Average Game Time (AGT)" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="33">
-      <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Games]]</calculatedColumnFormula>
-      <totalsRowFormula array="1">INT(Averages[Average Game Time (AGT)])&amp;" minutes"</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{0AA5346B-236D-4E0F-BA60-5AB0FC09F6C3}" name="Average Round Time (ART)" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
+      <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Rounds]]</calculatedColumnFormula>
+      <totalsRowFormula array="1">INT(Averages[Average Round Time (ART)])&amp;" minutes"</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E04C1373-75E0-4A6C-A2C9-4AA9B2CD365B}" name="Points Per Game (PPG)" dataDxfId="32">
-      <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Games]]</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{E04C1373-75E0-4A6C-A2C9-4AA9B2CD365B}" name="Points Per Round (PPR)" dataDxfId="21">
+      <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Rounds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{89B46B09-6052-4D3C-AAEC-F9A7E8580516}" name="Minutes Per Point (MPP)" dataDxfId="31">
+    <tableColumn id="4" xr3:uid="{89B46B09-6052-4D3C-AAEC-F9A7E8580516}" name="Minutes Per Point (MPP)" dataDxfId="20">
       <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Points]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{728FBC8B-7DB9-4E00-BB6D-2AFFBA13751D}" name="Points Per Minute (PPM)" dataDxfId="30">
+    <tableColumn id="3" xr3:uid="{728FBC8B-7DB9-4E00-BB6D-2AFFBA13751D}" name="Points Per Minute (PPM)" dataDxfId="19">
       <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Playtime (Minutes)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -422,7 +394,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}" name="November6" displayName="November6" ref="A2:E25" totalsRowCount="1" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}" name="November6" displayName="November6" ref="A2:E25" totalsRowCount="1" headerRowDxfId="18">
   <autoFilter ref="A2:E24" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -431,16 +403,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{366B94B4-B5FA-4886-9257-E9412E290946}" name="Points" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="27">
+    <tableColumn id="1" xr3:uid="{366B94B4-B5FA-4886-9257-E9412E290946}" name="Points" totalsRowFunction="custom" dataDxfId="17">
       <totalsRowFormula>SUM(November6[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{73EA15C4-D270-483C-AF4F-24B0B93502DB}" name="Games" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="25">
+    <tableColumn id="2" xr3:uid="{73EA15C4-D270-483C-AF4F-24B0B93502DB}" name="Rounds" totalsRowFunction="custom" dataDxfId="16">
       <calculatedColumnFormula array="1">_xlfn.IFS(November6[[#This Row],[Points]]=2, 1, November6[[#This Row],[Points]]=6, 2, November6[[#This Row],[Points]]=14, 3, November6[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
-      <totalsRowFormula>SUM(November6[Games])</totalsRowFormula>
+      <totalsRowFormula>SUM(November6[Rounds])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B3F474C8-DDEB-4DBF-A1DC-4AFC668AED9D}" name="Start Time" totalsRowDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{8665BCD7-C389-46C0-8A10-F495D85709FF}" name="End Time" totalsRowDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{5DE48718-2A9C-4594-A3FE-0C43DCAFF2C2}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="22">
+    <tableColumn id="4" xr3:uid="{B3F474C8-DDEB-4DBF-A1DC-4AFC668AED9D}" name="Start Time"/>
+    <tableColumn id="5" xr3:uid="{8665BCD7-C389-46C0-8A10-F495D85709FF}" name="End Time"/>
+    <tableColumn id="6" xr3:uid="{5DE48718-2A9C-4594-A3FE-0C43DCAFF2C2}" name="Playtime (Minutes)" totalsRowFunction="custom">
       <calculatedColumnFormula xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November6[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -450,7 +422,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}" name="November7" displayName="November7" ref="H2:L9" totalsRowCount="1" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}" name="November7" displayName="November7" ref="H2:L9" totalsRowCount="1" headerRowDxfId="15">
   <autoFilter ref="H2:L8" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -459,16 +431,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F89E074E-4750-48A3-A073-819989626FA6}" name="Points" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
+    <tableColumn id="1" xr3:uid="{F89E074E-4750-48A3-A073-819989626FA6}" name="Points" totalsRowFunction="custom" dataDxfId="14">
       <totalsRowFormula>SUM(November7[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D7CDB5A2-50B5-4939-8668-1785714D08C7}" name="Games" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="17">
+    <tableColumn id="2" xr3:uid="{D7CDB5A2-50B5-4939-8668-1785714D08C7}" name="Rounds" totalsRowFunction="custom" dataDxfId="13">
       <calculatedColumnFormula array="1">_xlfn.IFS(November7[[#This Row],[Points]]=2, 1, November7[[#This Row],[Points]]=6, 2, November7[[#This Row],[Points]]=14, 3, November7[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
-      <totalsRowFormula>SUM(November7[Games])</totalsRowFormula>
+      <totalsRowFormula>SUM(November7[Rounds])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28309402-7EF3-454D-883F-D251D524A71A}" name="Start Time" totalsRowDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{74A71E4E-B89F-47C8-B7A2-E5012A8EEFF3}" name="End Time" totalsRowDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{5610F31C-E244-4937-8B69-B467C9F24C5D}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="14">
+    <tableColumn id="4" xr3:uid="{28309402-7EF3-454D-883F-D251D524A71A}" name="Start Time"/>
+    <tableColumn id="5" xr3:uid="{74A71E4E-B89F-47C8-B7A2-E5012A8EEFF3}" name="End Time"/>
+    <tableColumn id="6" xr3:uid="{5610F31C-E244-4937-8B69-B467C9F24C5D}" name="Playtime (Minutes)" totalsRowFunction="custom">
       <calculatedColumnFormula xml:space="preserve"> (INT(November7[[#This Row],[End Time]]/100)*60 + MOD(November7[[#This Row],[End Time]],100)) - (INT(November7[[#This Row],[Start Time]]/100)*60 + MOD(November7[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November7[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -478,7 +450,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}" name="November9" displayName="November9" ref="O2:S13" totalsRowCount="1" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}" name="November9" displayName="November9" ref="O2:S13" totalsRowCount="1" headerRowDxfId="12">
   <autoFilter ref="O2:S12" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -487,16 +459,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CDE914EB-DF9D-42C8-A121-6BDB5A6D584A}" name="Points" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="1" xr3:uid="{CDE914EB-DF9D-42C8-A121-6BDB5A6D584A}" name="Points" totalsRowFunction="custom" dataDxfId="11">
       <totalsRowFormula>SUM(November9[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{423C97EA-A31A-446C-BECE-2F0330150ABC}" name="Games" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="9">
+    <tableColumn id="2" xr3:uid="{423C97EA-A31A-446C-BECE-2F0330150ABC}" name="Rounds" totalsRowFunction="custom" dataDxfId="10">
       <calculatedColumnFormula array="1">_xlfn.IFS(November9[[#This Row],[Points]]=2, 1, November9[[#This Row],[Points]]=6, 2, November9[[#This Row],[Points]]=14, 3, November9[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
-      <totalsRowFormula>SUM(November9[Games])</totalsRowFormula>
+      <totalsRowFormula>SUM(November9[Rounds])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C922EE3A-46E9-42C2-B0FC-BF56A61D0BD7}" name="Start Time" totalsRowDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{6E1643A5-7328-4CFF-9BB2-C0C48B9C9925}" name="End Time" totalsRowDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{F4DDC90C-E19C-46A6-93D1-39B9313C9028}" name="Playtime (Minutes)" totalsRowFunction="custom" totalsRowDxfId="6">
+    <tableColumn id="4" xr3:uid="{C922EE3A-46E9-42C2-B0FC-BF56A61D0BD7}" name="Start Time"/>
+    <tableColumn id="5" xr3:uid="{6E1643A5-7328-4CFF-9BB2-C0C48B9C9925}" name="End Time"/>
+    <tableColumn id="6" xr3:uid="{F4DDC90C-E19C-46A6-93D1-39B9313C9028}" name="Playtime (Minutes)" totalsRowFunction="custom">
       <calculatedColumnFormula xml:space="preserve"> (INT(November9[[#This Row],[End Time]]/100)*60 + MOD(November9[[#This Row],[End Time]],100)) - (INT(November9[[#This Row],[Start Time]]/100)*60 + MOD(November9[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November9[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
@@ -506,7 +478,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}" name="November10" displayName="November10" ref="V2:Z11" totalsRowCount="1" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}" name="November10" displayName="November10" ref="V2:Z11" totalsRowCount="1" headerRowDxfId="9">
   <autoFilter ref="V2:Z10" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -515,12 +487,12 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{82DBC3F1-720E-42A7-9B61-D5995B025F92}" name="Points" totalsRowFunction="custom" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{82DBC3F1-720E-42A7-9B61-D5995B025F92}" name="Points" totalsRowFunction="custom" dataDxfId="8">
       <totalsRowFormula>SUM(November10[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D4B36161-B381-44F4-8DD1-C5FEFF82C827}" name="Games" totalsRowFunction="custom" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{D4B36161-B381-44F4-8DD1-C5FEFF82C827}" name="Rounds" totalsRowFunction="custom" dataDxfId="7">
       <calculatedColumnFormula array="1">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
-      <totalsRowFormula>SUM(November10[Games])</totalsRowFormula>
+      <totalsRowFormula>SUM(November10[Rounds])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F8CE62ED-FE69-4019-BE42-B64F0A253950}" name="Start Time"/>
     <tableColumn id="5" xr3:uid="{504A287C-496D-4EBC-8784-5941FCB774D0}" name="End Time"/>
@@ -534,7 +506,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}" name="November11" displayName="November11" ref="AC2:AG7" totalsRowCount="1" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}" name="November11" displayName="November11" ref="AC2:AG7" totalsRowCount="1" headerRowDxfId="6">
   <autoFilter ref="AC2:AG6" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -543,18 +515,46 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{17F8BEAD-5484-4181-AD6E-07482D69DE92}" name="Points" totalsRowFunction="custom" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{17F8BEAD-5484-4181-AD6E-07482D69DE92}" name="Points" totalsRowFunction="custom" dataDxfId="5">
       <totalsRowFormula>SUM(November11[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B6CD6212-DA43-4D8D-86AB-D2A238A82270}" name="Games" totalsRowFunction="custom" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{B6CD6212-DA43-4D8D-86AB-D2A238A82270}" name="Rounds" totalsRowFunction="custom" dataDxfId="4">
       <calculatedColumnFormula array="1">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
-      <totalsRowFormula>SUM(November11[Games])</totalsRowFormula>
+      <totalsRowFormula>SUM(November11[Rounds])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{398AD5BB-5E5F-4DE7-A1C9-5C90562A08F8}" name="Start Time"/>
     <tableColumn id="5" xr3:uid="{681F54AF-8DAF-4DFE-8FBC-A274A6DB355A}" name="End Time"/>
     <tableColumn id="6" xr3:uid="{99CB9CF4-605E-4FB4-A631-BF5DB7AAAD86}" name="Playtime (Minutes)" totalsRowFunction="custom">
       <calculatedColumnFormula xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November11[Playtime (Minutes)])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2E053F8C-7BD7-43CB-9CBA-E4E1D9355DEA}" name="November12" displayName="November12" ref="AJ2:AN19" totalsRowCount="1" headerRowDxfId="3">
+  <autoFilter ref="AJ2:AN18" xr:uid="{2E053F8C-7BD7-43CB-9CBA-E4E1D9355DEA}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B44E0D43-C8A0-4D85-856E-A7D2DC9B8D3D}" name="Points" totalsRowFunction="custom" dataDxfId="2">
+      <totalsRowFormula>SUM(November12[Points])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{C285507D-7F2E-494A-B18F-9751931ED2F2}" name="Rounds" totalsRowFunction="custom" dataDxfId="1">
+      <calculatedColumnFormula array="1">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
+      <totalsRowFormula>SUM(November12[Rounds])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{703F9882-8D0B-4566-A4D1-DC01436CB3A3}" name="Start Time"/>
+    <tableColumn id="5" xr3:uid="{EA54BF8D-F878-4E3F-8BE9-79266C12F399}" name="End Time"/>
+    <tableColumn id="6" xr3:uid="{857A8EAE-ABC1-4607-94B3-5B1D8E129D98}" name="Playtime (Minutes)" totalsRowFunction="custom">
+      <calculatedColumnFormula xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</calculatedColumnFormula>
+      <totalsRowFormula>SUM(November12[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
@@ -824,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,40 +844,40 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <f>November6[[#Totals],[Points]]</f>
         <v>141</v>
       </c>
       <c r="C2">
-        <f>IFERROR(November6[[#Totals],[Games]], 0)</f>
+        <f>IFERROR(November6[[#Totals],[Rounds]], 0)</f>
         <v>34</v>
       </c>
       <c r="D2">
@@ -885,32 +885,32 @@
         <v>445</v>
       </c>
       <c r="G2" s="1">
-        <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Games]]</f>
-        <v>12.705263157894738</v>
+        <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Rounds]]</f>
+        <v>12.708333333333334</v>
       </c>
       <c r="H2" s="1">
-        <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Games]]</f>
-        <v>4.8947368421052628</v>
+        <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Rounds]]</f>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I2" s="1">
         <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Points]]</f>
-        <v>2.5956989247311828</v>
+        <v>2.76268115942029</v>
       </c>
       <c r="J2" s="1">
         <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Playtime (Minutes)]]</f>
-        <v>0.38525269262634632</v>
+        <v>0.3619672131147541</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <f>November7[[#Totals],[Points]]</f>
         <v>59</v>
       </c>
       <c r="C3">
-        <f>IFERROR(November7[[#Totals],[Games]], 0)</f>
+        <f>IFERROR(November7[[#Totals],[Rounds]], 0)</f>
         <v>13</v>
       </c>
       <c r="D3">
@@ -918,7 +918,7 @@
         <v>169</v>
       </c>
       <c r="G3" s="1" t="str" cm="1">
-        <f t="array" ref="G3">INT(Averages[Average Game Time (AGT)])&amp;" minutes"</f>
+        <f t="array" ref="G3">INT(Averages[Average Round Time (ART)])&amp;" minutes"</f>
         <v>12 minutes</v>
       </c>
       <c r="I3" s="1" t="str" cm="1">
@@ -928,14 +928,14 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <f>November9[[#Totals],[Points]]</f>
         <v>71</v>
       </c>
       <c r="C4">
-        <f>IFERROR(November9[[#Totals],[Games]], 0)</f>
+        <f>IFERROR(November9[[#Totals],[Rounds]], 0)</f>
         <v>18</v>
       </c>
       <c r="D4">
@@ -945,14 +945,14 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <f>November10[[#Totals],[Points]]</f>
         <v>159</v>
       </c>
       <c r="C5">
-        <f>IFERROR(November10[[#Totals],[Games]], 0)</f>
+        <f>IFERROR(November10[[#Totals],[Rounds]], 0)</f>
         <v>23</v>
       </c>
       <c r="D5">
@@ -962,14 +962,14 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <f>November11[[#Totals],[Points]]</f>
         <v>35</v>
       </c>
       <c r="C6">
-        <f>IFERROR(November11[[#Totals],[Games]], 0)</f>
+        <f>IFERROR(November11[[#Totals],[Rounds]], 0)</f>
         <v>7</v>
       </c>
       <c r="D6">
@@ -978,26 +978,43 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
+      <c r="A7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B7">
+        <f>November12[[#Totals],[Points]]</f>
+        <v>87</v>
+      </c>
+      <c r="C7" s="4">
+        <f>IFERROR(November12[[#Totals],[Rounds]], 0)</f>
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <f>November12[[#Totals],[Playtime (Minutes)]]</f>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <f>SUM(Totals[Total Points])</f>
-        <v>465</v>
-      </c>
-      <c r="C7">
-        <f>SUM(Totals[Total Games])</f>
-        <v>95</v>
-      </c>
-      <c r="D7">
+        <v>552</v>
+      </c>
+      <c r="C8">
+        <f>SUM(Totals[Total Rounds])</f>
+        <v>120</v>
+      </c>
+      <c r="D8">
         <f>SUM(Totals[Total Playtime (Minutes)])</f>
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="str">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="str">
         <f>INT(Totals[[#Totals],[Total Playtime (Minutes)]]/60)&amp;" hours  "&amp;INT(MOD(Totals[[#Totals],[Total Playtime (Minutes)]],60))&amp;" minutes"</f>
-        <v>20 hours  7 minutes</v>
+        <v>25 hours  25 minutes</v>
       </c>
     </row>
   </sheetData>
@@ -1007,10 +1024,11 @@
     <hyperlink ref="A4" location="DailyData!O1" display="November 9th" xr:uid="{9704D6B7-14DF-4C2C-BF93-C2230CF59ADA}"/>
     <hyperlink ref="A5" location="DailyData!V1" display="November 10th" xr:uid="{1B3FB756-63A6-46A9-8116-BFE00142D22A}"/>
     <hyperlink ref="A6" location="DailyData!AC1" display="November 11th" xr:uid="{323360C2-27FA-4A82-B965-6C0D4578D900}"/>
+    <hyperlink ref="A7" location="DailyData!AJ1" display="November 12th" xr:uid="{A96A6C91-2AD1-4ACB-8C3D-DB67BA8A4289}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C5:C6 C2:C4" calculatedColumn="1"/>
+    <ignoredError sqref="C5:C7 C2:C4" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
@@ -1021,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9762EC57-E733-40D9-8A42-9901A7D36B8F}">
-  <dimension ref="A1:AG30"/>
+  <dimension ref="A1:AN30"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AF13" sqref="AF13"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AO19" sqref="AO19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,123 +1071,150 @@
     <col min="31" max="31" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="23" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="H1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="O1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="V1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
       <c r="AC1" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="3"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1255,8 +1300,25 @@
         <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ3">
+        <v>2</v>
+      </c>
+      <c r="AK3" cm="1">
+        <f t="array" ref="AK3">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>1557</v>
+      </c>
+      <c r="AM3">
+        <v>2115</v>
+      </c>
+      <c r="AN3">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1319,10 +1381,10 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>33</v>
       </c>
-      <c r="AC4" s="4">
-        <v>2</v>
-      </c>
-      <c r="AD4" s="5" cm="1">
+      <c r="AC4">
+        <v>2</v>
+      </c>
+      <c r="AD4" cm="1">
         <f t="array" ref="AD4">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -1330,8 +1392,19 @@
         <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK4" s="6" cm="1">
+        <f t="array" ref="AK4">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN4">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
@@ -1376,10 +1449,10 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="AC5" s="4">
+      <c r="AC5">
         <v>25</v>
       </c>
-      <c r="AD5" s="5" cm="1">
+      <c r="AD5" cm="1">
         <f t="array" ref="AD5">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
@@ -1387,8 +1460,19 @@
         <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ5" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="6" cm="1">
+        <f t="array" ref="AK5">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN5">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1433,10 +1517,10 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="AC6" s="4">
+      <c r="AC6">
         <v>6</v>
       </c>
-      <c r="AD6" s="5" cm="1">
+      <c r="AD6" cm="1">
         <f t="array" ref="AD6">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</f>
         <v>2</v>
       </c>
@@ -1444,8 +1528,19 @@
         <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ6" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK6" s="6" cm="1">
+        <f t="array" ref="AK6">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN6">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14</v>
       </c>
@@ -1495,15 +1590,26 @@
         <v>35</v>
       </c>
       <c r="AD7">
-        <f>SUM(November11[Games])</f>
+        <f>SUM(November11[Rounds])</f>
         <v>7</v>
       </c>
       <c r="AG7">
         <f>SUM(November11[Playtime (Minutes)])</f>
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ7" s="5">
+        <v>14</v>
+      </c>
+      <c r="AK7" s="6" cm="1">
+        <f t="array" ref="AK7">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AN7">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1549,23 +1655,34 @@
         <v>0</v>
       </c>
       <c r="AC8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD8" t="s">
         <v>21</v>
       </c>
-      <c r="AD8" t="s">
-        <v>14</v>
-      </c>
       <c r="AE8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AF8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AG8" s="1" t="str">
         <f>INT(November11[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November11[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>1 hrs  30 mins</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ8" s="5">
+        <v>6</v>
+      </c>
+      <c r="AK8" s="6" cm="1">
+        <f t="array" ref="AK8">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AN8">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1582,7 +1699,7 @@
         <v>59</v>
       </c>
       <c r="I9">
-        <f>SUM(November7[Games])</f>
+        <f>SUM(November7[Rounds])</f>
         <v>13</v>
       </c>
       <c r="L9">
@@ -1612,11 +1729,11 @@
         <v>0</v>
       </c>
       <c r="AC9">
-        <f>November11[[#Totals],[Playtime (Minutes)]]/November11[[#Totals],[Games]]</f>
+        <f>November11[[#Totals],[Playtime (Minutes)]]/November11[[#Totals],[Rounds]]</f>
         <v>12.857142857142858</v>
       </c>
       <c r="AD9">
-        <f>November11[[#Totals],[Points]]/November11[[#Totals],[Games]]</f>
+        <f>November11[[#Totals],[Points]]/November11[[#Totals],[Rounds]]</f>
         <v>5</v>
       </c>
       <c r="AE9">
@@ -1627,8 +1744,19 @@
         <f>November11[[#Totals],[Points]]/November11[[#Totals],[Playtime (Minutes)]]</f>
         <v>0.3888888888888889</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ9" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK9" s="6" cm="1">
+        <f t="array" ref="AK9">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN9">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1641,16 +1769,16 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
         <v>21</v>
       </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
       <c r="J10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L10" s="1" t="str">
         <f>INT(November7[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November7[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
@@ -1678,8 +1806,19 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ10" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK10" s="6" cm="1">
+        <f t="array" ref="AK10">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1692,11 +1831,11 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <f>November7[[#Totals],[Playtime (Minutes)]]/November7[[#Totals],[Games]]</f>
+        <f>November7[[#Totals],[Playtime (Minutes)]]/November7[[#Totals],[Rounds]]</f>
         <v>13</v>
       </c>
       <c r="I11">
-        <f>November7[[#Totals],[Points]]/November7[[#Totals],[Games]]</f>
+        <f>November7[[#Totals],[Points]]/November7[[#Totals],[Rounds]]</f>
         <v>4.5384615384615383</v>
       </c>
       <c r="J11">
@@ -1723,7 +1862,7 @@
         <v>159</v>
       </c>
       <c r="W11">
-        <f>SUM(November10[Games])</f>
+        <f>SUM(November10[Rounds])</f>
         <v>23</v>
       </c>
       <c r="Z11">
@@ -1731,13 +1870,24 @@
         <v>271</v>
       </c>
       <c r="AC11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="AD11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="AJ11" s="5">
+        <v>6</v>
+      </c>
+      <c r="AK11" s="6" cm="1">
+        <f t="array" ref="AK11">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AN11">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1761,16 +1911,16 @@
         <v>0</v>
       </c>
       <c r="V12" t="s">
+        <v>19</v>
+      </c>
+      <c r="W12" t="s">
         <v>21</v>
       </c>
-      <c r="W12" t="s">
-        <v>14</v>
-      </c>
       <c r="X12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Y12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Z12" s="1" t="str">
         <f>INT(November10[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November10[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
@@ -1784,8 +1934,19 @@
         <f>November11[[#Totals],[Points]]/ROWS(November11[Points])</f>
         <v>8.75</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ12" s="5">
+        <v>25</v>
+      </c>
+      <c r="AK12" s="6" cm="1">
+        <f t="array" ref="AK12">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AN12">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1798,17 +1959,17 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O13">
         <f>SUM(November9[Points])</f>
         <v>71</v>
       </c>
       <c r="P13">
-        <f>SUM(November9[Games])</f>
+        <f>SUM(November9[Rounds])</f>
         <v>18</v>
       </c>
       <c r="S13">
@@ -1816,11 +1977,11 @@
         <v>232</v>
       </c>
       <c r="V13">
-        <f>November10[[#Totals],[Playtime (Minutes)]]/November10[[#Totals],[Games]]</f>
+        <f>November10[[#Totals],[Playtime (Minutes)]]/November10[[#Totals],[Rounds]]</f>
         <v>11.782608695652174</v>
       </c>
       <c r="W13">
-        <f>November10[[#Totals],[Points]]/November10[[#Totals],[Games]]</f>
+        <f>November10[[#Totals],[Points]]/November10[[#Totals],[Rounds]]</f>
         <v>6.9130434782608692</v>
       </c>
       <c r="X13">
@@ -1831,8 +1992,19 @@
         <f>November10[[#Totals],[Points]]/November10[[#Totals],[Playtime (Minutes)]]</f>
         <v>0.58671586715867163</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ13" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK13" s="6" cm="1">
+        <f t="array" ref="AK13">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN13">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1853,23 +2025,34 @@
         <v>9.8333333333333339</v>
       </c>
       <c r="O14" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" t="s">
         <v>21</v>
       </c>
-      <c r="P14" t="s">
-        <v>14</v>
-      </c>
       <c r="Q14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="S14" s="1" t="str">
         <f>INT(November9[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November9[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>3 hrs  52 mins</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AJ14" s="5">
+        <v>6</v>
+      </c>
+      <c r="AK14" s="6" cm="1">
+        <f t="array" ref="AK14">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AN14">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1882,11 +2065,11 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <f>November9[[#Totals],[Playtime (Minutes)]]/November9[[#Totals],[Games]]</f>
+        <f>November9[[#Totals],[Playtime (Minutes)]]/November9[[#Totals],[Rounds]]</f>
         <v>12.888888888888889</v>
       </c>
       <c r="P15">
-        <f>November9[[#Totals],[Points]]/November9[[#Totals],[Games]]</f>
+        <f>November9[[#Totals],[Points]]/November9[[#Totals],[Rounds]]</f>
         <v>3.9444444444444446</v>
       </c>
       <c r="Q15">
@@ -1898,13 +2081,24 @@
         <v>0.30603448275862066</v>
       </c>
       <c r="V15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="W15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="AJ15" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK15" s="6" cm="1">
+        <f t="array" ref="AK15">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN15">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1924,8 +2118,19 @@
         <f>November10[[#Totals],[Points]]/ROWS(November10[Points])</f>
         <v>19.875</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="AJ16" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK16" s="6" cm="1">
+        <f t="array" ref="AK16">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AN16">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1938,13 +2143,24 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="P17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="AJ17" s="5">
+        <v>6</v>
+      </c>
+      <c r="AK17" s="6" cm="1">
+        <f t="array" ref="AK17">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AN17">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1964,8 +2180,19 @@
         <f>November9[[#Totals],[Points]]/ROWS(November9[Points])</f>
         <v>7.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="AJ18" s="5">
+        <v>6</v>
+      </c>
+      <c r="AK18" s="6" cm="1">
+        <f t="array" ref="AK18">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AN18">
+        <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1977,8 +2204,20 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="AJ19">
+        <f>SUM(November12[Points])</f>
+        <v>87</v>
+      </c>
+      <c r="AK19">
+        <f>SUM(November12[Rounds])</f>
+        <v>25</v>
+      </c>
+      <c r="AN19">
+        <f>SUM(November12[Playtime (Minutes)])</f>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1990,8 +2229,24 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="AJ20" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN20" s="1" t="str">
+        <f>INT(November12[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November12[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
+        <v>5 hrs  18 mins</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -2003,8 +2258,24 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="AJ21">
+        <f>November12[[#Totals],[Playtime (Minutes)]]/November12[[#Totals],[Rounds]]</f>
+        <v>12.72</v>
+      </c>
+      <c r="AK21">
+        <f>November12[[#Totals],[Points]]/November12[[#Totals],[Rounds]]</f>
+        <v>3.48</v>
+      </c>
+      <c r="AL21">
+        <f>November12[[#Totals],[Playtime (Minutes)]]/November12[[#Totals],[Points]]</f>
+        <v>3.6551724137931036</v>
+      </c>
+      <c r="AM21">
+        <f>November12[[#Totals],[Points]]/November12[[#Totals],[Playtime (Minutes)]]</f>
+        <v>0.27358490566037735</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2017,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2029,8 +2300,14 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="AJ23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
@@ -2042,14 +2319,22 @@
         <f xml:space="preserve"> (INT(November6[[#This Row],[End Time]]/100)*60 + MOD(November6[[#This Row],[End Time]],100)) - (INT(November6[[#This Row],[Start Time]]/100)*60 + MOD(November6[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="AJ24">
+        <f>ROWS(November12[Points])</f>
+        <v>16</v>
+      </c>
+      <c r="AK24">
+        <f>November12[[#Totals],[Points]]/ROWS(November12[Points])</f>
+        <v>5.4375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>SUM(November6[Points])</f>
         <v>141</v>
       </c>
       <c r="B25">
-        <f>SUM(November6[Games])</f>
+        <f>SUM(November6[Rounds])</f>
         <v>34</v>
       </c>
       <c r="E25">
@@ -2057,31 +2342,31 @@
         <v>445</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
         <v>21</v>
       </c>
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="str">
         <f>INT(November6[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November6[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>7 hrs  25 mins</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>November6[[#Totals],[Playtime (Minutes)]]/November6[[#Totals],[Games]]</f>
+        <f>November6[[#Totals],[Playtime (Minutes)]]/November6[[#Totals],[Rounds]]</f>
         <v>13.088235294117647</v>
       </c>
       <c r="B27">
-        <f>November6[[#Totals],[Points]]/November6[[#Totals],[Games]]</f>
+        <f>November6[[#Totals],[Points]]/November6[[#Totals],[Rounds]]</f>
         <v>4.1470588235294121</v>
       </c>
       <c r="C27">
@@ -2093,15 +2378,15 @@
         <v>0.31685393258426964</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>ROWS(November6[Points])</f>
         <v>22</v>
@@ -2112,7 +2397,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="O1:S1"/>
@@ -2122,12 +2408,13 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more data and setup for next data gathering.
</commit_message>
<xml_diff>
--- a/Data/TheFINALS_Points.xlsx
+++ b/Data/TheFINALS_Points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GitHub\THE_FINALS-WorldTour-Calculator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673E1585-9EC4-4CDB-BB26-5714202D7679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D61052-53AB-4A10-95F8-83EC8BEB5321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="28">
   <si>
     <t>Total Points</t>
   </si>
@@ -138,6 +138,12 @@
   <si>
     <t>PPMatch</t>
   </si>
+  <si>
+    <t>November 13th</t>
+  </si>
+  <si>
+    <t>November 14th</t>
+  </si>
 </sst>
 </file>
 
@@ -211,9 +217,29 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="32">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -342,8 +368,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C27E572-866D-47E4-922E-826821481817}" name="Totals" displayName="Totals" ref="A1:D8" totalsRowCount="1" headerRowDxfId="25">
-  <autoFilter ref="A1:D7" xr:uid="{4C27E572-866D-47E4-922E-826821481817}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C27E572-866D-47E4-922E-826821481817}" name="Totals" displayName="Totals" ref="A1:D10" totalsRowCount="1" headerRowDxfId="31">
+  <autoFilter ref="A1:D9" xr:uid="{4C27E572-866D-47E4-922E-826821481817}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -355,7 +381,7 @@
       <totalsRowFormula>SUM(Totals[Total Points])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{40664CBD-E414-475B-A65B-20BCE21DEF0B}" name="Total Rounds" totalsRowFunction="custom" dataDxfId="0">
-      <calculatedColumnFormula>November6[[#Totals],[Points]]</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(November13[[#Totals],[Rounds]], 0)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Totals[Total Rounds])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C8AFE569-EB2B-4A94-8C17-1CF5EACFA5C3}" name="Total Playtime (Minutes)" totalsRowFunction="custom">
@@ -366,8 +392,36 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8E58F841-D8BB-4AA6-B725-7DE6FA828AF5}" name="November14" displayName="November14" ref="AX2:BB4" totalsRowCount="1" headerRowDxfId="3">
+  <autoFilter ref="AX2:BB3" xr:uid="{8E58F841-D8BB-4AA6-B725-7DE6FA828AF5}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A8194F85-4108-4BE5-BC58-1016594E7430}" name="Points" totalsRowFunction="custom" dataDxfId="2">
+      <totalsRowFormula>SUM(November14[Points])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{51F95EA8-D423-47AC-946C-C7A135B390EE}" name="Rounds" totalsRowFunction="custom" dataDxfId="1">
+      <calculatedColumnFormula array="1">_xlfn.IFS(November14[[#This Row],[Points]]=2, 1, November14[[#This Row],[Points]]=6, 2, November14[[#This Row],[Points]]=14, 3, November14[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
+      <totalsRowFormula>SUM(November14[Rounds])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{EED3DFB0-C13C-499F-97C6-B55167AA8306}" name="Start Time"/>
+    <tableColumn id="5" xr3:uid="{A4ED742E-CED0-49D1-A801-A3DA974E66BC}" name="End Time"/>
+    <tableColumn id="6" xr3:uid="{86D7929F-38C4-43C9-B7BD-08ED843D1E05}" name="Playtime (Minutes)" totalsRowFunction="custom">
+      <calculatedColumnFormula xml:space="preserve"> (INT(November14[[#This Row],[End Time]]/100)*60 + MOD(November14[[#This Row],[End Time]],100)) - (INT(November14[[#This Row],[Start Time]]/100)*60 + MOD(November14[[#This Row],[Start Time]],100))</calculatedColumnFormula>
+      <totalsRowFormula>SUM(November14[Playtime (Minutes)])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}" name="Averages" displayName="Averages" ref="G1:J2" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}" name="Averages" displayName="Averages" ref="G1:J2" headerRowDxfId="30">
   <autoFilter ref="G1:J2" xr:uid="{AF357DF9-4640-4E28-806E-EB6DD52A5BE7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -375,17 +429,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0AA5346B-236D-4E0F-BA60-5AB0FC09F6C3}" name="Average Round Time (ART)" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="1" xr3:uid="{0AA5346B-236D-4E0F-BA60-5AB0FC09F6C3}" name="Average Round Time (ART)" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
       <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Rounds]]</calculatedColumnFormula>
       <totalsRowFormula array="1">INT(Averages[Average Round Time (ART)])&amp;" minutes"</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E04C1373-75E0-4A6C-A2C9-4AA9B2CD365B}" name="Points Per Round (PPR)" dataDxfId="21">
+    <tableColumn id="2" xr3:uid="{E04C1373-75E0-4A6C-A2C9-4AA9B2CD365B}" name="Points Per Round (PPR)" dataDxfId="27">
       <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Rounds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{89B46B09-6052-4D3C-AAEC-F9A7E8580516}" name="Minutes Per Point (MPP)" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{89B46B09-6052-4D3C-AAEC-F9A7E8580516}" name="Minutes Per Point (MPP)" dataDxfId="26">
       <calculatedColumnFormula>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Points]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{728FBC8B-7DB9-4E00-BB6D-2AFFBA13751D}" name="Points Per Minute (PPM)" dataDxfId="19">
+    <tableColumn id="3" xr3:uid="{728FBC8B-7DB9-4E00-BB6D-2AFFBA13751D}" name="Points Per Minute (PPM)" dataDxfId="25">
       <calculatedColumnFormula>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Playtime (Minutes)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -394,7 +448,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}" name="November6" displayName="November6" ref="A2:E25" totalsRowCount="1" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}" name="November6" displayName="November6" ref="A2:E25" totalsRowCount="1" headerRowDxfId="24">
   <autoFilter ref="A2:E24" xr:uid="{EC6AD1EE-0CE2-409C-A2F6-F4A610CA243E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -403,10 +457,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{366B94B4-B5FA-4886-9257-E9412E290946}" name="Points" totalsRowFunction="custom" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{366B94B4-B5FA-4886-9257-E9412E290946}" name="Points" totalsRowFunction="custom" dataDxfId="23">
       <totalsRowFormula>SUM(November6[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{73EA15C4-D270-483C-AF4F-24B0B93502DB}" name="Rounds" totalsRowFunction="custom" dataDxfId="16">
+    <tableColumn id="2" xr3:uid="{73EA15C4-D270-483C-AF4F-24B0B93502DB}" name="Rounds" totalsRowFunction="custom" dataDxfId="22">
       <calculatedColumnFormula array="1">_xlfn.IFS(November6[[#This Row],[Points]]=2, 1, November6[[#This Row],[Points]]=6, 2, November6[[#This Row],[Points]]=14, 3, November6[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November6[Rounds])</totalsRowFormula>
     </tableColumn>
@@ -422,7 +476,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}" name="November7" displayName="November7" ref="H2:L9" totalsRowCount="1" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}" name="November7" displayName="November7" ref="H2:L9" totalsRowCount="1" headerRowDxfId="21">
   <autoFilter ref="H2:L8" xr:uid="{661DD5A8-F444-41F1-96C1-7AE436664A9D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -431,10 +485,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F89E074E-4750-48A3-A073-819989626FA6}" name="Points" totalsRowFunction="custom" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{F89E074E-4750-48A3-A073-819989626FA6}" name="Points" totalsRowFunction="custom" dataDxfId="20">
       <totalsRowFormula>SUM(November7[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D7CDB5A2-50B5-4939-8668-1785714D08C7}" name="Rounds" totalsRowFunction="custom" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{D7CDB5A2-50B5-4939-8668-1785714D08C7}" name="Rounds" totalsRowFunction="custom" dataDxfId="19">
       <calculatedColumnFormula array="1">_xlfn.IFS(November7[[#This Row],[Points]]=2, 1, November7[[#This Row],[Points]]=6, 2, November7[[#This Row],[Points]]=14, 3, November7[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November7[Rounds])</totalsRowFormula>
     </tableColumn>
@@ -450,7 +504,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}" name="November9" displayName="November9" ref="O2:S13" totalsRowCount="1" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}" name="November9" displayName="November9" ref="O2:S13" totalsRowCount="1" headerRowDxfId="18">
   <autoFilter ref="O2:S12" xr:uid="{E65DD4E2-B7B0-4DFF-9A0B-14FA157A8394}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -459,10 +513,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CDE914EB-DF9D-42C8-A121-6BDB5A6D584A}" name="Points" totalsRowFunction="custom" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{CDE914EB-DF9D-42C8-A121-6BDB5A6D584A}" name="Points" totalsRowFunction="custom" dataDxfId="17">
       <totalsRowFormula>SUM(November9[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{423C97EA-A31A-446C-BECE-2F0330150ABC}" name="Rounds" totalsRowFunction="custom" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{423C97EA-A31A-446C-BECE-2F0330150ABC}" name="Rounds" totalsRowFunction="custom" dataDxfId="16">
       <calculatedColumnFormula array="1">_xlfn.IFS(November9[[#This Row],[Points]]=2, 1, November9[[#This Row],[Points]]=6, 2, November9[[#This Row],[Points]]=14, 3, November9[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November9[Rounds])</totalsRowFormula>
     </tableColumn>
@@ -478,7 +532,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}" name="November10" displayName="November10" ref="V2:Z11" totalsRowCount="1" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}" name="November10" displayName="November10" ref="V2:Z11" totalsRowCount="1" headerRowDxfId="15">
   <autoFilter ref="V2:Z10" xr:uid="{B3490359-7E08-4CA3-9F95-FAFBADB3E82F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -487,10 +541,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{82DBC3F1-720E-42A7-9B61-D5995B025F92}" name="Points" totalsRowFunction="custom" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{82DBC3F1-720E-42A7-9B61-D5995B025F92}" name="Points" totalsRowFunction="custom" dataDxfId="14">
       <totalsRowFormula>SUM(November10[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D4B36161-B381-44F4-8DD1-C5FEFF82C827}" name="Rounds" totalsRowFunction="custom" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{D4B36161-B381-44F4-8DD1-C5FEFF82C827}" name="Rounds" totalsRowFunction="custom" dataDxfId="13">
       <calculatedColumnFormula array="1">_xlfn.IFS(November10[[#This Row],[Points]]=2, 1, November10[[#This Row],[Points]]=6, 2, November10[[#This Row],[Points]]=14, 3, November10[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November10[Rounds])</totalsRowFormula>
     </tableColumn>
@@ -506,7 +560,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}" name="November11" displayName="November11" ref="AC2:AG7" totalsRowCount="1" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}" name="November11" displayName="November11" ref="AC2:AG7" totalsRowCount="1" headerRowDxfId="12">
   <autoFilter ref="AC2:AG6" xr:uid="{128D98C7-5073-4B1B-8860-C9156B8B47F0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -515,10 +569,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{17F8BEAD-5484-4181-AD6E-07482D69DE92}" name="Points" totalsRowFunction="custom" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{17F8BEAD-5484-4181-AD6E-07482D69DE92}" name="Points" totalsRowFunction="custom" dataDxfId="11">
       <totalsRowFormula>SUM(November11[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B6CD6212-DA43-4D8D-86AB-D2A238A82270}" name="Rounds" totalsRowFunction="custom" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{B6CD6212-DA43-4D8D-86AB-D2A238A82270}" name="Rounds" totalsRowFunction="custom" dataDxfId="10">
       <calculatedColumnFormula array="1">_xlfn.IFS(November11[[#This Row],[Points]]=2, 1, November11[[#This Row],[Points]]=6, 2, November11[[#This Row],[Points]]=14, 3, November11[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November11[Rounds])</totalsRowFormula>
     </tableColumn>
@@ -534,7 +588,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2E053F8C-7BD7-43CB-9CBA-E4E1D9355DEA}" name="November12" displayName="November12" ref="AJ2:AN19" totalsRowCount="1" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2E053F8C-7BD7-43CB-9CBA-E4E1D9355DEA}" name="November12" displayName="November12" ref="AJ2:AN19" totalsRowCount="1" headerRowDxfId="9">
   <autoFilter ref="AJ2:AN18" xr:uid="{2E053F8C-7BD7-43CB-9CBA-E4E1D9355DEA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -543,10 +597,10 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B44E0D43-C8A0-4D85-856E-A7D2DC9B8D3D}" name="Points" totalsRowFunction="custom" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{B44E0D43-C8A0-4D85-856E-A7D2DC9B8D3D}" name="Points" totalsRowFunction="custom" dataDxfId="8">
       <totalsRowFormula>SUM(November12[Points])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C285507D-7F2E-494A-B18F-9751931ED2F2}" name="Rounds" totalsRowFunction="custom" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{C285507D-7F2E-494A-B18F-9751931ED2F2}" name="Rounds" totalsRowFunction="custom" dataDxfId="7">
       <calculatedColumnFormula array="1">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
       <totalsRowFormula>SUM(November12[Rounds])</totalsRowFormula>
     </tableColumn>
@@ -555,6 +609,34 @@
     <tableColumn id="6" xr3:uid="{857A8EAE-ABC1-4607-94B3-5B1D8E129D98}" name="Playtime (Minutes)" totalsRowFunction="custom">
       <calculatedColumnFormula xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</calculatedColumnFormula>
       <totalsRowFormula>SUM(November12[Playtime (Minutes)])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{66EA2851-D40B-4621-A548-428F858BF40E}" name="November13" displayName="November13" ref="AQ2:AU16" totalsRowCount="1" headerRowDxfId="6">
+  <autoFilter ref="AQ2:AU15" xr:uid="{66EA2851-D40B-4621-A548-428F858BF40E}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F1BE7FA5-47B4-462A-8F53-AA0791913209}" name="Points" totalsRowFunction="custom" dataDxfId="5">
+      <totalsRowFormula>SUM(November13[Points])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{2C623B63-3D4E-4DF4-871D-3F754E725E68}" name="Rounds" totalsRowFunction="custom" dataDxfId="4">
+      <calculatedColumnFormula array="1">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</calculatedColumnFormula>
+      <totalsRowFormula>SUM(November13[Rounds])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{4BBDF829-D46D-4CEC-A2CB-BFCE9DE14B9E}" name="Start Time"/>
+    <tableColumn id="5" xr3:uid="{E67391B4-D665-4DFB-9C8C-E4835D9B9B76}" name="End Time"/>
+    <tableColumn id="6" xr3:uid="{9B6E2D42-8CB5-44B8-A74D-1F7126F1C4CA}" name="Playtime (Minutes)" totalsRowFunction="custom">
+      <calculatedColumnFormula xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</calculatedColumnFormula>
+      <totalsRowFormula>SUM(November13[Playtime (Minutes)])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
@@ -824,16 +906,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
@@ -886,19 +967,19 @@
       </c>
       <c r="G2" s="1">
         <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Rounds]]</f>
-        <v>12.708333333333334</v>
+        <v>12.571428571428571</v>
       </c>
       <c r="H2" s="1">
         <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Rounds]]</f>
-        <v>4.5999999999999996</v>
+        <v>4.5238095238095237</v>
       </c>
       <c r="I2" s="1">
         <f>Totals[[#Totals],[Total Playtime (Minutes)]]/Totals[[#Totals],[Total Points]]</f>
-        <v>2.76268115942029</v>
+        <v>2.7789473684210528</v>
       </c>
       <c r="J2" s="1">
         <f>Totals[[#Totals],[Total Points]]/Totals[[#Totals],[Total Playtime (Minutes)]]</f>
-        <v>0.3619672131147541</v>
+        <v>0.35984848484848486</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -985,7 +1066,7 @@
         <f>November12[[#Totals],[Points]]</f>
         <v>87</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <f>IFERROR(November12[[#Totals],[Rounds]], 0)</f>
         <v>25</v>
       </c>
@@ -995,26 +1076,60 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
+      <c r="A8" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B8">
+        <f>November13[[#Totals],[Points]]</f>
+        <v>113</v>
+      </c>
+      <c r="C8" s="4">
+        <f>IFERROR(November13[[#Totals],[Rounds]], 0)</f>
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <f>November13[[#Totals],[Playtime (Minutes)]]</f>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <f>November14[[#Totals],[Points]]</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <f>IFERROR(November14[[#Totals],[Rounds]], 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>November14[[#Totals],[Playtime (Minutes)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <f>SUM(Totals[Total Points])</f>
-        <v>552</v>
-      </c>
-      <c r="C8">
+        <v>665</v>
+      </c>
+      <c r="C10">
         <f>SUM(Totals[Total Rounds])</f>
-        <v>120</v>
-      </c>
-      <c r="D8">
+        <v>147</v>
+      </c>
+      <c r="D10">
         <f>SUM(Totals[Total Playtime (Minutes)])</f>
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="str">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="str">
         <f>INT(Totals[[#Totals],[Total Playtime (Minutes)]]/60)&amp;" hours  "&amp;INT(MOD(Totals[[#Totals],[Total Playtime (Minutes)]],60))&amp;" minutes"</f>
-        <v>25 hours  25 minutes</v>
+        <v>30 hours  48 minutes</v>
       </c>
     </row>
   </sheetData>
@@ -1025,10 +1140,12 @@
     <hyperlink ref="A5" location="DailyData!V1" display="November 10th" xr:uid="{1B3FB756-63A6-46A9-8116-BFE00142D22A}"/>
     <hyperlink ref="A6" location="DailyData!AC1" display="November 11th" xr:uid="{323360C2-27FA-4A82-B965-6C0D4578D900}"/>
     <hyperlink ref="A7" location="DailyData!AJ1" display="November 12th" xr:uid="{A96A6C91-2AD1-4ACB-8C3D-DB67BA8A4289}"/>
+    <hyperlink ref="A8" location="DailyData!AQ1" display="November 13th" xr:uid="{17428DA0-3A3C-4008-92D6-A980BD6BBACE}"/>
+    <hyperlink ref="A9" location="DailyData!AX1" display="November 14th" xr:uid="{750A93DB-125B-4603-9136-6FCADA398269}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C5:C7 C2:C4" calculatedColumn="1"/>
+    <ignoredError sqref="C2:C6 C7:C9" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
@@ -1039,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9762EC57-E733-40D9-8A42-9901A7D36B8F}">
-  <dimension ref="A1:AN30"/>
+  <dimension ref="A1:BB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AO19" sqref="AO19"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1:BB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,9 +1193,19 @@
     <col min="38" max="38" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="23" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="23" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1121,8 +1248,22 @@
       <c r="AL1" s="3"/>
       <c r="AM1" s="3"/>
       <c r="AN1" s="3"/>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="AX1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3"/>
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1213,8 +1354,38 @@
       <c r="AN2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1317,8 +1488,33 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>318</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ3">
+        <v>2</v>
+      </c>
+      <c r="AR3" cm="1">
+        <f t="array" ref="AR3">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>1457</v>
+      </c>
+      <c r="AT3">
+        <v>2020</v>
+      </c>
+      <c r="AU3">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>323</v>
+      </c>
+      <c r="AY3" t="e" cm="1">
+        <f t="array" ref="AY3">_xlfn.IFS(November14[[#This Row],[Points]]=2, 1, November14[[#This Row],[Points]]=6, 2, November14[[#This Row],[Points]]=14, 3, November14[[#This Row],[Points]]=25, 3)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BB3">
+        <f xml:space="preserve"> (INT(November14[[#This Row],[End Time]]/100)*60 + MOD(November14[[#This Row],[End Time]],100)) - (INT(November14[[#This Row],[Start Time]]/100)*60 + MOD(November14[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1392,10 +1588,10 @@
         <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="AJ4" s="5">
-        <v>2</v>
-      </c>
-      <c r="AK4" s="6" cm="1">
+      <c r="AJ4">
+        <v>2</v>
+      </c>
+      <c r="AK4" cm="1">
         <f t="array" ref="AK4">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -1403,8 +1599,31 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ4" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR4" s="6" cm="1">
+        <f t="array" ref="AR4">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AU4">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <f>SUM(November14[Points])</f>
+        <v>0</v>
+      </c>
+      <c r="AY4" t="e">
+        <f>SUM(November14[Rounds])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="BB4">
+        <f>SUM(November14[Playtime (Minutes)])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
@@ -1460,10 +1679,10 @@
         <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="AJ5" s="5">
-        <v>2</v>
-      </c>
-      <c r="AK5" s="6" cm="1">
+      <c r="AJ5">
+        <v>2</v>
+      </c>
+      <c r="AK5" cm="1">
         <f t="array" ref="AK5">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -1471,8 +1690,35 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ5" s="5">
+        <v>14</v>
+      </c>
+      <c r="AR5" s="6" cm="1">
+        <f t="array" ref="AR5">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AU5">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>12</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB5" s="1" t="str">
+        <f>INT(November14[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November14[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
+        <v>0 hrs  0 mins</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1528,10 +1774,10 @@
         <f xml:space="preserve"> (INT(November11[[#This Row],[End Time]]/100)*60 + MOD(November11[[#This Row],[End Time]],100)) - (INT(November11[[#This Row],[Start Time]]/100)*60 + MOD(November11[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="5">
-        <v>2</v>
-      </c>
-      <c r="AK6" s="6" cm="1">
+      <c r="AJ6">
+        <v>2</v>
+      </c>
+      <c r="AK6" cm="1">
         <f t="array" ref="AK6">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -1539,8 +1785,35 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR6" s="6" cm="1">
+        <f t="array" ref="AR6">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AU6">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+      <c r="AX6" t="e">
+        <f>November14[[#Totals],[Playtime (Minutes)]]/November14[[#Totals],[Rounds]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AY6" t="e">
+        <f>November14[[#Totals],[Points]]/November14[[#Totals],[Rounds]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AZ6" t="e">
+        <f>November14[[#Totals],[Playtime (Minutes)]]/November14[[#Totals],[Points]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BA6" t="e">
+        <f>November14[[#Totals],[Points]]/November14[[#Totals],[Playtime (Minutes)]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14</v>
       </c>
@@ -1597,10 +1870,10 @@
         <f>SUM(November11[Playtime (Minutes)])</f>
         <v>90</v>
       </c>
-      <c r="AJ7" s="5">
+      <c r="AJ7">
         <v>14</v>
       </c>
-      <c r="AK7" s="6" cm="1">
+      <c r="AK7" cm="1">
         <f t="array" ref="AK7">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
@@ -1608,8 +1881,19 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ7" s="5">
+        <v>14</v>
+      </c>
+      <c r="AR7" s="6" cm="1">
+        <f t="array" ref="AR7">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AU7">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1670,10 +1954,10 @@
         <f>INT(November11[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November11[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>1 hrs  30 mins</v>
       </c>
-      <c r="AJ8" s="5">
-        <v>6</v>
-      </c>
-      <c r="AK8" s="6" cm="1">
+      <c r="AJ8">
+        <v>6</v>
+      </c>
+      <c r="AK8" cm="1">
         <f t="array" ref="AK8">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>2</v>
       </c>
@@ -1681,8 +1965,25 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ8" s="5">
+        <v>25</v>
+      </c>
+      <c r="AR8" s="6" cm="1">
+        <f t="array" ref="AR8">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AU8">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1744,10 +2045,10 @@
         <f>November11[[#Totals],[Points]]/November11[[#Totals],[Playtime (Minutes)]]</f>
         <v>0.3888888888888889</v>
       </c>
-      <c r="AJ9" s="5">
-        <v>2</v>
-      </c>
-      <c r="AK9" s="6" cm="1">
+      <c r="AJ9">
+        <v>2</v>
+      </c>
+      <c r="AK9" cm="1">
         <f t="array" ref="AK9">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -1755,8 +2056,27 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ9" s="5">
+        <v>14</v>
+      </c>
+      <c r="AR9" s="6" cm="1">
+        <f t="array" ref="AR9">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AU9">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <f>ROWS(November14[Points])</f>
+        <v>1</v>
+      </c>
+      <c r="AY9">
+        <f>November14[[#Totals],[Points]]/ROWS(November14[Points])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1806,10 +2126,10 @@
         <f xml:space="preserve"> (INT(November10[[#This Row],[End Time]]/100)*60 + MOD(November10[[#This Row],[End Time]],100)) - (INT(November10[[#This Row],[Start Time]]/100)*60 + MOD(November10[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-      <c r="AJ10" s="5">
-        <v>2</v>
-      </c>
-      <c r="AK10" s="6" cm="1">
+      <c r="AJ10">
+        <v>2</v>
+      </c>
+      <c r="AK10" cm="1">
         <f t="array" ref="AK10">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -1817,8 +2137,19 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ10" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR10" s="6" cm="1">
+        <f t="array" ref="AR10">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AU10">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1875,10 +2206,10 @@
       <c r="AD11" t="s">
         <v>13</v>
       </c>
-      <c r="AJ11" s="5">
-        <v>6</v>
-      </c>
-      <c r="AK11" s="6" cm="1">
+      <c r="AJ11">
+        <v>6</v>
+      </c>
+      <c r="AK11" cm="1">
         <f t="array" ref="AK11">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>2</v>
       </c>
@@ -1886,8 +2217,19 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ11" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR11" s="6" cm="1">
+        <f t="array" ref="AR11">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="AU11">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1934,10 +2276,10 @@
         <f>November11[[#Totals],[Points]]/ROWS(November11[Points])</f>
         <v>8.75</v>
       </c>
-      <c r="AJ12" s="5">
+      <c r="AJ12">
         <v>25</v>
       </c>
-      <c r="AK12" s="6" cm="1">
+      <c r="AK12" cm="1">
         <f t="array" ref="AK12">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>3</v>
       </c>
@@ -1945,8 +2287,19 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ12" s="5">
+        <v>14</v>
+      </c>
+      <c r="AR12" s="6" cm="1">
+        <f t="array" ref="AR12">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>3</v>
+      </c>
+      <c r="AU12">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1992,10 +2345,10 @@
         <f>November10[[#Totals],[Points]]/November10[[#Totals],[Playtime (Minutes)]]</f>
         <v>0.58671586715867163</v>
       </c>
-      <c r="AJ13" s="5">
-        <v>2</v>
-      </c>
-      <c r="AK13" s="6" cm="1">
+      <c r="AJ13">
+        <v>2</v>
+      </c>
+      <c r="AK13" cm="1">
         <f t="array" ref="AK13">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -2003,8 +2356,19 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ13" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR13" s="6" cm="1">
+        <f t="array" ref="AR13">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AU13">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -2040,10 +2404,10 @@
         <f>INT(November9[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November9[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>3 hrs  52 mins</v>
       </c>
-      <c r="AJ14" s="5">
-        <v>6</v>
-      </c>
-      <c r="AK14" s="6" cm="1">
+      <c r="AJ14">
+        <v>6</v>
+      </c>
+      <c r="AK14" cm="1">
         <f t="array" ref="AK14">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>2</v>
       </c>
@@ -2051,8 +2415,19 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ14" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR14" s="6" cm="1">
+        <f t="array" ref="AR14">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AU14">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2086,10 +2461,10 @@
       <c r="W15" t="s">
         <v>25</v>
       </c>
-      <c r="AJ15" s="5">
-        <v>2</v>
-      </c>
-      <c r="AK15" s="6" cm="1">
+      <c r="AJ15">
+        <v>2</v>
+      </c>
+      <c r="AK15" cm="1">
         <f t="array" ref="AK15">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -2097,8 +2472,19 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ15" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR15" s="6" cm="1">
+        <f t="array" ref="AR15">_xlfn.IFS(November13[[#This Row],[Points]]=2, 1, November13[[#This Row],[Points]]=6, 2, November13[[#This Row],[Points]]=14, 3, November13[[#This Row],[Points]]=25, 3)</f>
+        <v>2</v>
+      </c>
+      <c r="AU15">
+        <f xml:space="preserve"> (INT(November13[[#This Row],[End Time]]/100)*60 + MOD(November13[[#This Row],[End Time]],100)) - (INT(November13[[#This Row],[Start Time]]/100)*60 + MOD(November13[[#This Row],[Start Time]],100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2118,10 +2504,10 @@
         <f>November10[[#Totals],[Points]]/ROWS(November10[Points])</f>
         <v>19.875</v>
       </c>
-      <c r="AJ16" s="5">
-        <v>2</v>
-      </c>
-      <c r="AK16" s="6" cm="1">
+      <c r="AJ16">
+        <v>2</v>
+      </c>
+      <c r="AK16" cm="1">
         <f t="array" ref="AK16">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>1</v>
       </c>
@@ -2129,8 +2515,20 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ16">
+        <f>SUM(November13[Points])</f>
+        <v>113</v>
+      </c>
+      <c r="AR16">
+        <f>SUM(November13[Rounds])</f>
+        <v>27</v>
+      </c>
+      <c r="AU16">
+        <f>SUM(November13[Playtime (Minutes)])</f>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2148,10 +2546,10 @@
       <c r="P17" t="s">
         <v>13</v>
       </c>
-      <c r="AJ17" s="5">
-        <v>6</v>
-      </c>
-      <c r="AK17" s="6" cm="1">
+      <c r="AJ17">
+        <v>6</v>
+      </c>
+      <c r="AK17" cm="1">
         <f t="array" ref="AK17">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>2</v>
       </c>
@@ -2159,8 +2557,24 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU17" s="1" t="str">
+        <f>INT(November13[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November13[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
+        <v>5 hrs  23 mins</v>
+      </c>
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -2180,10 +2594,10 @@
         <f>November9[[#Totals],[Points]]/ROWS(November9[Points])</f>
         <v>7.1</v>
       </c>
-      <c r="AJ18" s="5">
-        <v>6</v>
-      </c>
-      <c r="AK18" s="6" cm="1">
+      <c r="AJ18">
+        <v>6</v>
+      </c>
+      <c r="AK18" cm="1">
         <f t="array" ref="AK18">_xlfn.IFS(November12[[#This Row],[Points]]=2, 1, November12[[#This Row],[Points]]=6, 2, November12[[#This Row],[Points]]=14, 3, November12[[#This Row],[Points]]=25, 3)</f>
         <v>2</v>
       </c>
@@ -2191,8 +2605,24 @@
         <f xml:space="preserve"> (INT(November12[[#This Row],[End Time]]/100)*60 + MOD(November12[[#This Row],[End Time]],100)) - (INT(November12[[#This Row],[Start Time]]/100)*60 + MOD(November12[[#This Row],[Start Time]],100))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ18">
+        <f>November13[[#Totals],[Playtime (Minutes)]]/November13[[#Totals],[Rounds]]</f>
+        <v>11.962962962962964</v>
+      </c>
+      <c r="AR18">
+        <f>November13[[#Totals],[Points]]/November13[[#Totals],[Rounds]]</f>
+        <v>4.1851851851851851</v>
+      </c>
+      <c r="AS18">
+        <f>November13[[#Totals],[Playtime (Minutes)]]/November13[[#Totals],[Points]]</f>
+        <v>2.8584070796460175</v>
+      </c>
+      <c r="AT18">
+        <f>November13[[#Totals],[Points]]/November13[[#Totals],[Playtime (Minutes)]]</f>
+        <v>0.34984520123839008</v>
+      </c>
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2217,7 +2647,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2245,8 +2675,14 @@
         <f>INT(November12[[#Totals],[Playtime (Minutes)]]/60)&amp;" hrs  "&amp;INT(MOD(November12[[#Totals],[Playtime (Minutes)]],60))&amp;" mins"</f>
         <v>5 hrs  18 mins</v>
       </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -2274,8 +2710,16 @@
         <f>November12[[#Totals],[Points]]/November12[[#Totals],[Playtime (Minutes)]]</f>
         <v>0.27358490566037735</v>
       </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ21">
+        <f>ROWS(November13[Points])</f>
+        <v>13</v>
+      </c>
+      <c r="AR21">
+        <f>November13[[#Totals],[Points]]/ROWS(November13[Points])</f>
+        <v>8.6923076923076916</v>
+      </c>
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2288,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2307,7 +2751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
@@ -2328,7 +2772,7 @@
         <v>5.4375</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>SUM(November6[Points])</f>
         <v>141</v>
@@ -2342,7 +2786,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2360,7 +2804,7 @@
         <v>7 hrs  25 mins</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>November6[[#Totals],[Playtime (Minutes)]]/November6[[#Totals],[Rounds]]</f>
         <v>13.088235294117647</v>
@@ -2378,7 +2822,7 @@
         <v>0.31685393258426964</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2386,7 +2830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>ROWS(November6[Points])</f>
         <v>22</v>
@@ -2397,7 +2841,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="AQ1:AU1"/>
+    <mergeCell ref="AX1:BB1"/>
     <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="H1:L1"/>
@@ -2408,13 +2854,15 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="6">
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>